<commit_message>
feat：update dragon excel change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Dragon_龙表.xlsx
+++ b/dragon-verse/Excels/Dragon_龙表.xlsx
@@ -1171,8 +1171,8 @@
   <sheetPr/>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5"/>
@@ -1309,7 +1309,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -1341,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
@@ -1373,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -1405,7 +1405,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
@@ -1437,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
@@ -1470,7 +1470,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
@@ -1503,7 +1503,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2">
         <v>1</v>
@@ -1536,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G12" s="2">
         <v>1</v>
@@ -1569,7 +1569,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
@@ -1602,7 +1602,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G14" s="2">
         <v>1</v>
@@ -1635,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
@@ -1668,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G16" s="2">
         <v>1</v>
@@ -1701,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
@@ -1733,7 +1733,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G18" s="2">
         <v>1</v>
@@ -1765,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
@@ -1797,7 +1797,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G20" s="2">
         <v>1</v>
@@ -1829,7 +1829,7 @@
         <v>3</v>
       </c>
       <c r="F21" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G21" s="2">
         <v>1</v>
@@ -1861,7 +1861,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G22" s="2">
         <v>1</v>
@@ -1893,7 +1893,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G23" s="2">
         <v>1</v>
@@ -1925,7 +1925,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G24" s="2">
         <v>1</v>
@@ -1957,7 +1957,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G25" s="2">
         <v>1</v>
@@ -1989,7 +1989,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G26" s="2">
         <v>1</v>
@@ -2021,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="F27" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G27" s="2">
         <v>1</v>
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="F28" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
@@ -2085,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="F29" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G29" s="2">
         <v>1</v>
@@ -2117,7 +2117,7 @@
         <v>3</v>
       </c>
       <c r="F30" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G30" s="2">
         <v>1</v>
@@ -2149,7 +2149,7 @@
         <v>3</v>
       </c>
       <c r="F31" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G31" s="2">
         <v>1</v>
@@ -2181,7 +2181,7 @@
         <v>3</v>
       </c>
       <c r="F32" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G32" s="2">
         <v>1</v>
@@ -2213,7 +2213,7 @@
         <v>3</v>
       </c>
       <c r="F33" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G33" s="2">
         <v>1</v>
@@ -2245,7 +2245,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G34" s="2">
         <v>1</v>
@@ -2277,7 +2277,7 @@
         <v>3</v>
       </c>
       <c r="F35" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G35" s="2">
         <v>1</v>
@@ -2309,7 +2309,7 @@
         <v>3</v>
       </c>
       <c r="F36" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G36" s="2">
         <v>1</v>
@@ -2341,7 +2341,7 @@
         <v>3</v>
       </c>
       <c r="F37" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G37" s="2">
         <v>1</v>
@@ -2373,7 +2373,7 @@
         <v>3</v>
       </c>
       <c r="F38" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G38" s="2">
         <v>1</v>
@@ -2405,7 +2405,7 @@
         <v>3</v>
       </c>
       <c r="F39" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G39" s="2">
         <v>1</v>
@@ -2437,7 +2437,7 @@
         <v>3</v>
       </c>
       <c r="F40" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G40" s="2">
         <v>1</v>
@@ -2469,7 +2469,7 @@
         <v>3</v>
       </c>
       <c r="F41" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G41" s="2">
         <v>1</v>
@@ -2501,7 +2501,7 @@
         <v>3</v>
       </c>
       <c r="F42" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G42" s="2">
         <v>1</v>
@@ -2533,7 +2533,7 @@
         <v>3</v>
       </c>
       <c r="F43" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G43" s="2">
         <v>1</v>
@@ -2565,7 +2565,7 @@
         <v>3</v>
       </c>
       <c r="F44" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G44" s="2">
         <v>1</v>
@@ -2597,7 +2597,7 @@
         <v>3</v>
       </c>
       <c r="F45" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G45" s="2">
         <v>1</v>
@@ -2629,7 +2629,7 @@
         <v>3</v>
       </c>
       <c r="F46" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G46" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
feat：udpate dragon wing change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Dragon_龙表.xlsx
+++ b/dragon-verse/Excels/Dragon_龙表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>int</t>
   </si>
@@ -134,30 +134,33 @@
     <t>15CE57BE4D934D8E09508BAD4D9CEF6F</t>
   </si>
   <si>
+    <t>0|0|0||0|0|90||1|1|1</t>
+  </si>
+  <si>
+    <t>F3BA53C9435F8BA3C26C7EB5BAF22C6E</t>
+  </si>
+  <si>
+    <t>34185B544D794914D28E14927DF8BF9D</t>
+  </si>
+  <si>
+    <t>1ECFFBAF4EB541264762CC890F968872</t>
+  </si>
+  <si>
+    <t>5039CCD64DA4F2FDFFC8A1A6FF303806</t>
+  </si>
+  <si>
+    <t>37D752654AD6C496BCB97797B16B32E6</t>
+  </si>
+  <si>
+    <t>8BD91D2A4219B36F850259A31B81BFF7</t>
+  </si>
+  <si>
+    <t>E59CCE1B4B573E9E89526D8713A6DD02</t>
+  </si>
+  <si>
     <t>0|0|0||0|0|0||1|1|1</t>
   </si>
   <si>
-    <t>F3BA53C9435F8BA3C26C7EB5BAF22C6E</t>
-  </si>
-  <si>
-    <t>34185B544D794914D28E14927DF8BF9D</t>
-  </si>
-  <si>
-    <t>1ECFFBAF4EB541264762CC890F968872</t>
-  </si>
-  <si>
-    <t>5039CCD64DA4F2FDFFC8A1A6FF303806</t>
-  </si>
-  <si>
-    <t>37D752654AD6C496BCB97797B16B32E6</t>
-  </si>
-  <si>
-    <t>8BD91D2A4219B36F850259A31B81BFF7</t>
-  </si>
-  <si>
-    <t>E59CCE1B4B573E9E89526D8713A6DD02</t>
-  </si>
-  <si>
     <t>ABD1639E4D7779781D8E3495D0B6C695</t>
   </si>
   <si>
@@ -212,9 +215,6 @@
     <t>A6DCDB104A426394C3ABD3ABA4FDF33F</t>
   </si>
   <si>
-    <t>0|0|0||0|0|-15||1|1|1</t>
-  </si>
-  <si>
     <t>90FA9C9A4B328B679FAC2BBFE5EB4C3D</t>
   </si>
   <si>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t>EA3E87F34584BB5A2952ED8C569D0466</t>
-  </si>
-  <si>
-    <t>0|0|0||0|0|90||1|1|1</t>
   </si>
   <si>
     <t>1358C5AF4D53BA31762373BDF951A5A9</t>
@@ -1171,8 +1168,8 @@
   <sheetPr/>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5"/>
@@ -1448,7 +1445,7 @@
       <c r="I9" s="8">
         <v>145909</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="8"/>
@@ -1481,7 +1478,7 @@
       <c r="I10" s="8">
         <v>145909</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K10" s="8"/>
@@ -1514,7 +1511,7 @@
       <c r="I11" s="8">
         <v>145909</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="8"/>
@@ -1777,7 +1774,7 @@
         <v>136963</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" spans="1:10">
@@ -1785,7 +1782,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" s="8">
         <v>19</v>
@@ -1809,7 +1806,7 @@
         <v>136963</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:10">
@@ -1817,7 +1814,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="7">
         <v>20</v>
@@ -1841,7 +1838,7 @@
         <v>136963</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" spans="1:10">
@@ -1849,7 +1846,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="7">
         <v>21</v>
@@ -1873,7 +1870,7 @@
         <v>136963</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" spans="1:10">
@@ -1881,7 +1878,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2">
         <v>22</v>
@@ -1905,7 +1902,7 @@
         <v>136963</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" spans="1:10">
@@ -1913,7 +1910,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2">
         <v>23</v>
@@ -1937,7 +1934,7 @@
         <v>136963</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" spans="1:10">
@@ -1945,7 +1942,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" s="2">
         <v>24</v>
@@ -1969,7 +1966,7 @@
         <v>136963</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" spans="1:10">
@@ -1977,7 +1974,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C26" s="8">
         <v>25</v>
@@ -2001,7 +1998,7 @@
         <v>136957</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" spans="1:10">
@@ -2009,7 +2006,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C27" s="8">
         <v>26</v>
@@ -2033,7 +2030,7 @@
         <v>42830</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" spans="1:10">
@@ -2041,7 +2038,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2">
         <v>27</v>
@@ -2065,7 +2062,7 @@
         <v>42830</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" spans="1:10">
@@ -2073,7 +2070,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2">
         <v>28</v>
@@ -2097,7 +2094,7 @@
         <v>136957</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" spans="1:10">
@@ -2105,7 +2102,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2">
         <v>29</v>
@@ -2129,7 +2126,7 @@
         <v>42825</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" spans="1:10">
@@ -2137,7 +2134,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" s="2">
         <v>30</v>
@@ -2161,7 +2158,7 @@
         <v>136957</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" spans="1:10">
@@ -2169,7 +2166,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32" s="2">
         <v>31</v>
@@ -2193,7 +2190,7 @@
         <v>42825</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" spans="1:10">
@@ -2201,7 +2198,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2">
         <v>32</v>
@@ -2225,7 +2222,7 @@
         <v>42829</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" spans="1:10">
@@ -2257,7 +2254,7 @@
         <v>42829</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" spans="1:10">
@@ -2289,7 +2286,7 @@
         <v>42829</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" s="2" customFormat="1" spans="1:10">
@@ -2321,7 +2318,7 @@
         <v>42829</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" s="2" customFormat="1" spans="1:10">
@@ -2353,7 +2350,7 @@
         <v>42829</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" s="2" customFormat="1" spans="1:10">
@@ -2385,7 +2382,7 @@
         <v>42829</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" s="2" customFormat="1" spans="1:10">
@@ -2417,7 +2414,7 @@
         <v>42829</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" s="2" customFormat="1" spans="1:10">
@@ -2449,7 +2446,7 @@
         <v>42813</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" s="2" customFormat="1" spans="1:10">
@@ -2457,7 +2454,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2">
         <v>40</v>
@@ -2481,7 +2478,7 @@
         <v>42813</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2489,7 +2486,7 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" s="2">
         <v>41</v>
@@ -2513,7 +2510,7 @@
         <v>42813</v>
       </c>
       <c r="J42" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2521,7 +2518,7 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="2">
         <v>42</v>
@@ -2545,7 +2542,7 @@
         <v>42813</v>
       </c>
       <c r="J43" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2553,7 +2550,7 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="2">
         <v>43</v>
@@ -2577,7 +2574,7 @@
         <v>42813</v>
       </c>
       <c r="J44" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2585,7 +2582,7 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="2">
         <v>44</v>
@@ -2609,7 +2606,7 @@
         <v>42813</v>
       </c>
       <c r="J45" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2617,7 +2614,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" s="2">
         <v>45</v>
@@ -2641,7 +2638,7 @@
         <v>42813</v>
       </c>
       <c r="J46" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update BagItem table
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Dragon_龙表.xlsx
+++ b/dragon-verse/Excels/Dragon_龙表.xlsx
@@ -1,33 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12375"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Constant" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames>
+    <definedName name="MaxCount" hidden="0">Constant!$B$1</definedName>
+  </definedNames>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>int</t>
   </si>
@@ -80,16 +70,16 @@
     <t>形象</t>
   </si>
   <si>
-    <t>背包物 ID</t>
-  </si>
-  <si>
-    <t>元素 ID</t>
-  </si>
-  <si>
-    <t>品质 ID</t>
-  </si>
-  <si>
-    <t>龙栖居地场景 ID</t>
+    <t xml:space="preserve">背包物 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">元素 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">品质 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">龙栖居地场景 ID</t>
   </si>
   <si>
     <t>可捕捉次数</t>
@@ -104,7 +94,7 @@
     <t>翅膀相对位置||旋转||缩放</t>
   </si>
   <si>
-    <t>捕捉成功率算法 ID</t>
+    <t xml:space="preserve">捕捉成功率算法 ID</t>
   </si>
   <si>
     <t>468E88AD49228BA4B2590DBE0E07ABDE</t>
@@ -255,173 +245,161 @@
   </si>
   <si>
     <t>B4D3185544BCCC8845FD53A24EACDAC9</t>
+  </si>
+  <si>
+    <t>MaxLanItemCount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="160" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="161" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="162" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="163" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
-      <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color indexed="4"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color indexed="20"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color indexed="2"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="18.000000"/>
       <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="15.000000"/>
       <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="13.000000"/>
       <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color indexed="65"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <name val="微软雅黑"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.000000"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
     </font>
   </fonts>
   <fills count="33">
@@ -481,20 +459,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor theme="4" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor theme="4" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.79998168889431398"/>
+        <bgColor theme="4" tint="0.79998168889431398"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810496"/>
+        <bgColor theme="4" tint="0.59999389629810496"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241899"/>
+        <bgColor theme="4" tint="0.39997558519241899"/>
       </patternFill>
     </fill>
     <fill>
@@ -505,20 +483,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor theme="5" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor theme="5" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.79998168889431398"/>
+        <bgColor theme="5" tint="0.79998168889431398"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810496"/>
+        <bgColor theme="5" tint="0.59999389629810496"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241899"/>
+        <bgColor theme="5" tint="0.39997558519241899"/>
       </patternFill>
     </fill>
     <fill>
@@ -529,20 +507,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor theme="6" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor theme="6" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.79998168889431398"/>
+        <bgColor theme="6" tint="0.79998168889431398"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810496"/>
+        <bgColor theme="6" tint="0.59999389629810496"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241899"/>
+        <bgColor theme="6" tint="0.39997558519241899"/>
       </patternFill>
     </fill>
     <fill>
@@ -553,20 +531,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor theme="7" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor theme="7" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.79998168889431398"/>
+        <bgColor theme="7" tint="0.79998168889431398"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810496"/>
+        <bgColor theme="7" tint="0.59999389629810496"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241899"/>
+        <bgColor theme="7" tint="0.39997558519241899"/>
       </patternFill>
     </fill>
     <fill>
@@ -577,20 +555,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor theme="8" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor theme="8" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.79998168889431398"/>
+        <bgColor theme="8" tint="0.79998168889431398"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810496"/>
+        <bgColor theme="8" tint="0.59999389629810496"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241899"/>
+        <bgColor theme="8" tint="0.39997558519241899"/>
       </patternFill>
     </fill>
     <fill>
@@ -601,30 +579,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor theme="9" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor theme="9" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.79998168889431398"/>
+        <bgColor theme="9" tint="0.79998168889431398"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810496"/>
+        <bgColor theme="9" tint="0.59999389629810496"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241899"/>
+        <bgColor theme="9" tint="0.39997558519241899"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="9">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -639,25 +617,25 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -672,7 +650,7 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -687,7 +665,7 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="double">
@@ -702,202 +680,203 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="none"/>
+      <right style="none"/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="161" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="162" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="163" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="7" fillId="0" borderId="2" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="2" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="3" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="10" fillId="3" borderId="4" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="11" fillId="4" borderId="5" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="12" fillId="4" borderId="4" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="13" fillId="5" borderId="6" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="14" fillId="0" borderId="7" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="15" fillId="0" borderId="8" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="16" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="17" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="18" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="10" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="11" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="12" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="13" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="14" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="15" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="16" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="17" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="18" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="19" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="20" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="21" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="22" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="23" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="24" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="25" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="26" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="27" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="28" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="29" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="30" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="31" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="19" fillId="32" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -950,6 +929,7 @@
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -959,8 +939,291 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1167,40 +1430,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:K46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="F50" activeCellId="0" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.625" customWidth="1"/>
-    <col min="6" max="6" width="22.375" customWidth="1"/>
-    <col min="9" max="9" width="17.125" customWidth="1"/>
-    <col min="10" max="10" width="23.625" customWidth="1"/>
-    <col min="11" max="11" width="17.125" customWidth="1"/>
+    <col customWidth="1" min="2" max="2" width="37.625"/>
+    <col customWidth="1" min="6" max="6" width="22.375"/>
+    <col customWidth="1" min="9" max="9" width="17.125"/>
+    <col customWidth="1" min="10" max="10" width="23.625"/>
+    <col customWidth="1" min="11" max="11" width="17.125"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1219,23 +1484,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:11">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="1" customFormat="1">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1254,7 +1519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:11">
+    <row r="3" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1264,7 +1529,7 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1289,17 +1554,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="4:4">
+    <row r="4" s="5" customFormat="1">
       <c r="D4" s="6"/>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:10">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" s="5" customFormat="1">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>4</v>
       </c>
       <c r="D5" s="6">
@@ -1308,27 +1573,27 @@
       <c r="E5" s="7">
         <v>3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="5">
         <v>6</v>
       </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
         <v>145909</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:10">
-      <c r="A6" s="2">
+    <row r="6" s="5" customFormat="1">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="7">
@@ -1340,27 +1605,27 @@
       <c r="E6" s="7">
         <v>3</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="5">
         <v>6</v>
       </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
         <v>145909</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="1" spans="1:10">
-      <c r="A7" s="2">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="7" s="5" customFormat="1">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="7">
@@ -1372,59 +1637,59 @@
       <c r="E7" s="7">
         <v>3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="5">
         <v>6</v>
       </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
         <v>145909</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="1" spans="1:10">
-      <c r="A8" s="2">
+    <row r="8" s="5" customFormat="1">
+      <c r="A8" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>7</v>
       </c>
       <c r="D8" s="6">
         <v>5</v>
       </c>
-      <c r="E8" s="2">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="5">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5">
         <v>6</v>
       </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
         <v>145909</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="1" spans="1:11">
-      <c r="A9" s="2">
+    <row r="9" s="5" customFormat="1">
+      <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="8">
@@ -1436,13 +1701,13 @@
       <c r="E9" s="7">
         <v>3</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="5">
         <v>6</v>
       </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
         <v>1</v>
       </c>
       <c r="I9" s="8">
@@ -1453,29 +1718,29 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" s="2" customFormat="1" spans="1:11">
-      <c r="A10" s="2">
+    <row r="10" s="5" customFormat="1">
+      <c r="A10" s="5">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>9</v>
       </c>
       <c r="D10" s="6">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
         <v>6</v>
       </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
         <v>1</v>
       </c>
       <c r="I10" s="8">
@@ -1486,11 +1751,11 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" s="2" customFormat="1" spans="1:11">
-      <c r="A11" s="2">
+    <row r="11" s="5" customFormat="1">
+      <c r="A11" s="5">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="7">
@@ -1502,13 +1767,13 @@
       <c r="E11" s="7">
         <v>3</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="5">
         <v>6</v>
       </c>
-      <c r="G11" s="2">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
         <v>1</v>
       </c>
       <c r="I11" s="8">
@@ -1519,11 +1784,11 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" s="2" customFormat="1" spans="1:11">
-      <c r="A12" s="2">
+    <row r="12" s="5" customFormat="1">
+      <c r="A12" s="5">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="7">
@@ -1538,10 +1803,10 @@
       <c r="F12" s="7">
         <v>7</v>
       </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
         <v>1</v>
       </c>
       <c r="I12" s="8">
@@ -1552,11 +1817,11 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" s="2" customFormat="1" spans="1:11">
-      <c r="A13" s="2">
+    <row r="13" s="5" customFormat="1">
+      <c r="A13" s="5">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="8">
@@ -1571,10 +1836,10 @@
       <c r="F13" s="7">
         <v>7</v>
       </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
         <v>1</v>
       </c>
       <c r="I13" s="8">
@@ -1585,11 +1850,11 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" s="2" customFormat="1" spans="1:11">
-      <c r="A14" s="2">
+    <row r="14" s="5" customFormat="1">
+      <c r="A14" s="5">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="8">
@@ -1604,10 +1869,10 @@
       <c r="F14" s="7">
         <v>7</v>
       </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
         <v>1</v>
       </c>
       <c r="I14" s="8">
@@ -1618,11 +1883,11 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" s="2" customFormat="1" spans="1:11">
-      <c r="A15" s="2">
+    <row r="15" s="5" customFormat="1">
+      <c r="A15" s="5">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="8">
@@ -1637,10 +1902,10 @@
       <c r="F15" s="7">
         <v>7</v>
       </c>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
         <v>1</v>
       </c>
       <c r="I15" s="8">
@@ -1651,11 +1916,11 @@
       </c>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" s="2" customFormat="1" spans="1:11">
-      <c r="A16" s="2">
+    <row r="16" s="5" customFormat="1">
+      <c r="A16" s="5">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="7">
@@ -1670,10 +1935,10 @@
       <c r="F16" s="7">
         <v>7</v>
       </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5">
         <v>1</v>
       </c>
       <c r="I16" s="8">
@@ -1684,11 +1949,11 @@
       </c>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" s="2" customFormat="1" spans="1:10">
-      <c r="A17" s="2">
+    <row r="17" s="5" customFormat="1">
+      <c r="A17" s="5">
         <v>13</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="7">
@@ -1703,10 +1968,10 @@
       <c r="F17" s="7">
         <v>7</v>
       </c>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
         <v>1</v>
       </c>
       <c r="I17" s="8">
@@ -1716,11 +1981,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" s="2" customFormat="1" spans="1:10">
-      <c r="A18" s="2">
+    <row r="18" s="5" customFormat="1">
+      <c r="A18" s="5">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="8">
@@ -1735,10 +2000,10 @@
       <c r="F18" s="7">
         <v>7</v>
       </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
         <v>1</v>
       </c>
       <c r="I18" s="8">
@@ -1748,11 +2013,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" spans="1:10">
-      <c r="A19" s="2">
+    <row r="19" s="5" customFormat="1">
+      <c r="A19" s="5">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="8">
@@ -1767,24 +2032,24 @@
       <c r="F19" s="7">
         <v>2</v>
       </c>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2">
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
         <v>136963</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" s="2" customFormat="1" spans="1:10">
-      <c r="A20" s="2">
+    <row r="20" s="5" customFormat="1">
+      <c r="A20" s="5">
         <v>16</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="8">
@@ -1799,24 +2064,24 @@
       <c r="F20" s="7">
         <v>2</v>
       </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
         <v>136963</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="1" spans="1:10">
-      <c r="A21" s="2">
+    <row r="21" s="5" customFormat="1">
+      <c r="A21" s="5">
         <v>17</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="7">
@@ -1831,24 +2096,24 @@
       <c r="F21" s="7">
         <v>2</v>
       </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
         <v>136963</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" s="2" customFormat="1" spans="1:10">
-      <c r="A22" s="2">
+    <row r="22" s="5" customFormat="1">
+      <c r="A22" s="5">
         <v>18</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="7">
@@ -1863,27 +2128,27 @@
       <c r="F22" s="7">
         <v>2</v>
       </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2">
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5">
         <v>136963</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" s="2" customFormat="1" spans="1:10">
-      <c r="A23" s="2">
+    <row r="23" s="5" customFormat="1">
+      <c r="A23" s="5">
         <v>19</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="5">
         <v>22</v>
       </c>
       <c r="D23" s="6">
@@ -1895,27 +2160,27 @@
       <c r="F23" s="7">
         <v>2</v>
       </c>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5">
         <v>136963</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" s="2" customFormat="1" spans="1:10">
-      <c r="A24" s="2">
+    <row r="24" s="5" customFormat="1">
+      <c r="A24" s="5">
         <v>20</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="5">
         <v>23</v>
       </c>
       <c r="D24" s="6">
@@ -1927,27 +2192,27 @@
       <c r="F24" s="7">
         <v>2</v>
       </c>
-      <c r="G24" s="2">
-        <v>1</v>
-      </c>
-      <c r="H24" s="2">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2">
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
         <v>136963</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" spans="1:10">
-      <c r="A25" s="2">
+    <row r="25" s="5" customFormat="1">
+      <c r="A25" s="5">
         <v>21</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="5">
         <v>24</v>
       </c>
       <c r="D25" s="6">
@@ -1959,24 +2224,24 @@
       <c r="F25" s="7">
         <v>2</v>
       </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2">
-        <v>1</v>
-      </c>
-      <c r="I25" s="2">
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
+      <c r="I25" s="5">
         <v>136963</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" s="2" customFormat="1" spans="1:10">
-      <c r="A26" s="2">
+    <row r="26" s="5" customFormat="1">
+      <c r="A26" s="5">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="8">
@@ -1991,24 +2256,24 @@
       <c r="F26" s="7">
         <v>3</v>
       </c>
-      <c r="G26" s="2">
-        <v>1</v>
-      </c>
-      <c r="H26" s="2">
-        <v>1</v>
-      </c>
-      <c r="I26" s="2">
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5">
         <v>136957</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" s="2" customFormat="1" spans="1:10">
-      <c r="A27" s="2">
+    <row r="27" s="5" customFormat="1">
+      <c r="A27" s="5">
         <v>23</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="8">
@@ -2023,27 +2288,27 @@
       <c r="F27" s="7">
         <v>3</v>
       </c>
-      <c r="G27" s="2">
-        <v>1</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="5">
         <v>42830</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" spans="1:10">
-      <c r="A28" s="2">
+    <row r="28" s="5" customFormat="1">
+      <c r="A28" s="5">
         <v>24</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="5">
         <v>27</v>
       </c>
       <c r="D28" s="6">
@@ -2055,27 +2320,27 @@
       <c r="F28" s="7">
         <v>3</v>
       </c>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2">
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5">
         <v>42830</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" s="2" customFormat="1" spans="1:10">
-      <c r="A29" s="2">
+    <row r="29" s="5" customFormat="1">
+      <c r="A29" s="5">
         <v>25</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="5">
         <v>28</v>
       </c>
       <c r="D29" s="6">
@@ -2087,27 +2352,27 @@
       <c r="F29" s="7">
         <v>3</v>
       </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5">
         <v>136957</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="1" spans="1:10">
-      <c r="A30" s="2">
+    <row r="30" s="5" customFormat="1">
+      <c r="A30" s="5">
         <v>26</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="5">
         <v>29</v>
       </c>
       <c r="D30" s="6">
@@ -2119,27 +2384,27 @@
       <c r="F30" s="7">
         <v>3</v>
       </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1</v>
-      </c>
-      <c r="I30" s="2">
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30" s="5">
         <v>42825</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" s="2" customFormat="1" spans="1:10">
-      <c r="A31" s="2">
+    <row r="31" s="5" customFormat="1">
+      <c r="A31" s="5">
         <v>27</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="5">
         <v>30</v>
       </c>
       <c r="D31" s="6">
@@ -2151,27 +2416,27 @@
       <c r="F31" s="7">
         <v>3</v>
       </c>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
         <v>136957</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" s="2" customFormat="1" spans="1:10">
-      <c r="A32" s="2">
+    <row r="32" s="5" customFormat="1">
+      <c r="A32" s="5">
         <v>28</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="5">
         <v>31</v>
       </c>
       <c r="D32" s="6">
@@ -2183,27 +2448,27 @@
       <c r="F32" s="7">
         <v>3</v>
       </c>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2">
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
+        <v>1</v>
+      </c>
+      <c r="I32" s="5">
         <v>42825</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" s="2" customFormat="1" spans="1:10">
-      <c r="A33" s="2">
+    <row r="33" s="5" customFormat="1">
+      <c r="A33" s="5">
         <v>29</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="5">
         <v>32</v>
       </c>
       <c r="D33" s="6">
@@ -2215,27 +2480,27 @@
       <c r="F33" s="7">
         <v>5</v>
       </c>
-      <c r="G33" s="2">
-        <v>1</v>
-      </c>
-      <c r="H33" s="2">
-        <v>1</v>
-      </c>
-      <c r="I33" s="2">
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5">
         <v>42829</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" s="2" customFormat="1" spans="1:10">
-      <c r="A34" s="2">
+    <row r="34" s="5" customFormat="1">
+      <c r="A34" s="5">
         <v>30</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="5">
         <v>33</v>
       </c>
       <c r="D34" s="6">
@@ -2247,27 +2512,27 @@
       <c r="F34" s="7">
         <v>5</v>
       </c>
-      <c r="G34" s="2">
-        <v>1</v>
-      </c>
-      <c r="H34" s="2">
-        <v>1</v>
-      </c>
-      <c r="I34" s="2">
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1</v>
+      </c>
+      <c r="I34" s="5">
         <v>42829</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" s="2" customFormat="1" spans="1:10">
-      <c r="A35" s="2">
+    <row r="35" s="5" customFormat="1">
+      <c r="A35" s="5">
         <v>31</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="5">
         <v>34</v>
       </c>
       <c r="D35" s="6">
@@ -2279,27 +2544,27 @@
       <c r="F35" s="7">
         <v>5</v>
       </c>
-      <c r="G35" s="2">
-        <v>1</v>
-      </c>
-      <c r="H35" s="2">
-        <v>1</v>
-      </c>
-      <c r="I35" s="2">
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5">
         <v>42829</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" s="2" customFormat="1" spans="1:10">
-      <c r="A36" s="2">
+    <row r="36" s="5" customFormat="1">
+      <c r="A36" s="5">
         <v>32</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="5">
         <v>35</v>
       </c>
       <c r="D36" s="6">
@@ -2311,27 +2576,27 @@
       <c r="F36" s="7">
         <v>5</v>
       </c>
-      <c r="G36" s="2">
-        <v>1</v>
-      </c>
-      <c r="H36" s="2">
-        <v>1</v>
-      </c>
-      <c r="I36" s="2">
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1</v>
+      </c>
+      <c r="I36" s="5">
         <v>42829</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" s="2" customFormat="1" spans="1:10">
-      <c r="A37" s="2">
+    <row r="37" s="5" customFormat="1">
+      <c r="A37" s="5">
         <v>33</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="5">
         <v>36</v>
       </c>
       <c r="D37" s="6">
@@ -2343,27 +2608,27 @@
       <c r="F37" s="7">
         <v>5</v>
       </c>
-      <c r="G37" s="2">
-        <v>1</v>
-      </c>
-      <c r="H37" s="2">
-        <v>1</v>
-      </c>
-      <c r="I37" s="2">
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>1</v>
+      </c>
+      <c r="I37" s="5">
         <v>42829</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" s="2" customFormat="1" spans="1:10">
-      <c r="A38" s="2">
+    <row r="38" s="5" customFormat="1">
+      <c r="A38" s="5">
         <v>34</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="5">
         <v>37</v>
       </c>
       <c r="D38" s="6">
@@ -2375,27 +2640,27 @@
       <c r="F38" s="7">
         <v>5</v>
       </c>
-      <c r="G38" s="2">
-        <v>1</v>
-      </c>
-      <c r="H38" s="2">
-        <v>1</v>
-      </c>
-      <c r="I38" s="2">
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
+      <c r="I38" s="5">
         <v>42829</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" s="2" customFormat="1" spans="1:10">
-      <c r="A39" s="2">
+    <row r="39" s="5" customFormat="1">
+      <c r="A39" s="5">
         <v>35</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="5">
         <v>38</v>
       </c>
       <c r="D39" s="6">
@@ -2407,27 +2672,27 @@
       <c r="F39" s="7">
         <v>5</v>
       </c>
-      <c r="G39" s="2">
-        <v>1</v>
-      </c>
-      <c r="H39" s="2">
-        <v>1</v>
-      </c>
-      <c r="I39" s="2">
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5">
         <v>42829</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" s="2" customFormat="1" spans="1:10">
-      <c r="A40" s="2">
+    <row r="40" s="5" customFormat="1">
+      <c r="A40" s="5">
         <v>36</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="5">
         <v>39</v>
       </c>
       <c r="D40" s="6">
@@ -2439,27 +2704,27 @@
       <c r="F40" s="7">
         <v>4</v>
       </c>
-      <c r="G40" s="2">
-        <v>1</v>
-      </c>
-      <c r="H40" s="2">
-        <v>1</v>
-      </c>
-      <c r="I40" s="2">
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5">
         <v>42813</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" s="2" customFormat="1" spans="1:10">
-      <c r="A41" s="2">
+    <row r="41" s="5" customFormat="1">
+      <c r="A41" s="5">
         <v>37</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="5">
         <v>40</v>
       </c>
       <c r="D41" s="6">
@@ -2471,27 +2736,27 @@
       <c r="F41" s="7">
         <v>4</v>
       </c>
-      <c r="G41" s="2">
-        <v>1</v>
-      </c>
-      <c r="H41" s="2">
-        <v>1</v>
-      </c>
-      <c r="I41" s="2">
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5">
         <v>42813</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="2">
+    <row r="42">
+      <c r="A42" s="5">
         <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="5">
         <v>41</v>
       </c>
       <c r="D42" s="6">
@@ -2503,27 +2768,27 @@
       <c r="F42" s="7">
         <v>4</v>
       </c>
-      <c r="G42" s="2">
-        <v>1</v>
-      </c>
-      <c r="H42" s="2">
-        <v>1</v>
-      </c>
-      <c r="I42" s="2">
+      <c r="G42" s="5">
+        <v>1</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42" s="5">
         <v>42813</v>
       </c>
       <c r="J42" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="2">
+    <row r="43">
+      <c r="A43" s="5">
         <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="5">
         <v>42</v>
       </c>
       <c r="D43" s="6">
@@ -2535,27 +2800,27 @@
       <c r="F43" s="7">
         <v>4</v>
       </c>
-      <c r="G43" s="2">
-        <v>1</v>
-      </c>
-      <c r="H43" s="2">
-        <v>1</v>
-      </c>
-      <c r="I43" s="2">
+      <c r="G43" s="5">
+        <v>1</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1</v>
+      </c>
+      <c r="I43" s="5">
         <v>42813</v>
       </c>
       <c r="J43" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="2">
+    <row r="44">
+      <c r="A44" s="5">
         <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="5">
         <v>43</v>
       </c>
       <c r="D44" s="6">
@@ -2567,27 +2832,27 @@
       <c r="F44" s="7">
         <v>4</v>
       </c>
-      <c r="G44" s="2">
-        <v>1</v>
-      </c>
-      <c r="H44" s="2">
-        <v>1</v>
-      </c>
-      <c r="I44" s="2">
+      <c r="G44" s="5">
+        <v>1</v>
+      </c>
+      <c r="H44" s="5">
+        <v>1</v>
+      </c>
+      <c r="I44" s="5">
         <v>42813</v>
       </c>
       <c r="J44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="2">
+    <row r="45">
+      <c r="A45" s="5">
         <v>41</v>
       </c>
       <c r="B45" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="5">
         <v>44</v>
       </c>
       <c r="D45" s="6">
@@ -2599,27 +2864,27 @@
       <c r="F45" s="7">
         <v>4</v>
       </c>
-      <c r="G45" s="2">
-        <v>1</v>
-      </c>
-      <c r="H45" s="2">
-        <v>1</v>
-      </c>
-      <c r="I45" s="2">
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
+      <c r="I45" s="5">
         <v>42813</v>
       </c>
       <c r="J45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="2">
+    <row r="46">
+      <c r="A46" s="5">
         <v>42</v>
       </c>
       <c r="B46" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="5">
         <v>45</v>
       </c>
       <c r="D46" s="6">
@@ -2631,13 +2896,13 @@
       <c r="F46" s="7">
         <v>4</v>
       </c>
-      <c r="G46" s="2">
-        <v>1</v>
-      </c>
-      <c r="H46" s="2">
-        <v>1</v>
-      </c>
-      <c r="I46" s="2">
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5">
+        <v>1</v>
+      </c>
+      <c r="I46" s="5">
         <v>42813</v>
       </c>
       <c r="J46" t="s">
@@ -2645,11 +2910,37 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.0249999999999997" bottom="1.0249999999999997" header="0.78750000000000009" footer="0.78750000000000009"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="1" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,标准"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,标准"页 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update Dragon table
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Dragon_龙表.xlsx
+++ b/dragon-verse/Excels/Dragon_龙表.xlsx
@@ -403,7 +403,7 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="5">
+        <row r="6">
           <cell r="D1" t="str">
             <v>string</v>
           </cell>
@@ -427,9 +427,13 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="5">
-          <cell r="B1"/>
-          <cell r="A1"/>
+        <row r="6">
+          <cell r="B1" t="str">
+            <v>string</v>
+          </cell>
+          <cell r="A1" t="str">
+            <v>int</v>
+          </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
@@ -1103,9 +1107,9 @@
       <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="10" t="e">
-        <f ca="1">MATCH($D5,OFFSET('[2]Sheet1'!$A$5,0,0,500),0)</f>
-        <v>#N/A</v>
+      <c r="C6" s="10" t="str">
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A6,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <v/>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1728,7 +1732,7 @@
         <v>53</v>
       </c>
       <c r="C22" s="10" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B22,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A22,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D22">
@@ -1767,7 +1771,7 @@
         <v>54</v>
       </c>
       <c r="C23" s="10" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B23,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A23,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D23">
@@ -1806,7 +1810,7 @@
         <v>55</v>
       </c>
       <c r="C24" s="10" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B24,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A24,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D24">
@@ -1845,7 +1849,7 @@
         <v>56</v>
       </c>
       <c r="C25" s="10" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B25,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A25,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D25">
@@ -1884,7 +1888,7 @@
         <v>57</v>
       </c>
       <c r="C26" s="10" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B26,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A26,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D26">
@@ -1923,7 +1927,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="10" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B27,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A27,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D27">
@@ -1962,7 +1966,7 @@
         <v>62</v>
       </c>
       <c r="C28" s="10" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B28,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A28,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D28">
@@ -2001,7 +2005,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B29,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A29,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D29">
@@ -2040,7 +2044,7 @@
         <v>65</v>
       </c>
       <c r="C30" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B30,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A30,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D30">
@@ -2079,7 +2083,7 @@
         <v>67</v>
       </c>
       <c r="C31" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B31,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A31,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D31">
@@ -2118,7 +2122,7 @@
         <v>68</v>
       </c>
       <c r="C32" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B32,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A32,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D32">
@@ -2157,7 +2161,7 @@
         <v>69</v>
       </c>
       <c r="C33" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B33,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A33,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D33">
@@ -2196,7 +2200,7 @@
         <v>71</v>
       </c>
       <c r="C34" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B34,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A34,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D34">
@@ -2235,7 +2239,7 @@
         <v>72</v>
       </c>
       <c r="C35" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B35,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A35,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D35">
@@ -2274,7 +2278,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B36,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A36,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D36">
@@ -2313,7 +2317,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B37,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A37,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D37">
@@ -2352,7 +2356,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B38,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A38,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D38">
@@ -2391,7 +2395,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B39,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A39,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D39">
@@ -2430,7 +2434,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B40,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A40,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D40">
@@ -2469,7 +2473,7 @@
         <v>79</v>
       </c>
       <c r="C41" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B41,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A41,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D41">
@@ -2508,7 +2512,7 @@
         <v>80</v>
       </c>
       <c r="C42" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B42,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A42,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D42">
@@ -2547,7 +2551,7 @@
         <v>81</v>
       </c>
       <c r="C43" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B43,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A43,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D43">
@@ -2586,7 +2590,7 @@
         <v>82</v>
       </c>
       <c r="C44" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B44,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A44,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D44">
@@ -2625,7 +2629,7 @@
         <v>83</v>
       </c>
       <c r="C45" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B45,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A45,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D45">
@@ -2664,7 +2668,7 @@
         <v>84</v>
       </c>
       <c r="C46" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B46,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A46,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D46">
@@ -2697,2725 +2701,2725 @@
     </row>
     <row r="47" ht="15">
       <c r="C47" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B47,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A47,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="48" ht="15">
       <c r="C48" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B48,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A48,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="49" ht="15">
       <c r="C49" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B49,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A49,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="50" ht="15">
       <c r="C50" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B50,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A50,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="51" ht="15">
       <c r="C51" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B51,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A51,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="52" ht="15">
       <c r="C52" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B52,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A52,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="53" ht="15">
       <c r="C53" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B53,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A53,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="54" ht="15">
       <c r="C54" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B54,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A54,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="55" ht="15">
       <c r="C55" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B55,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A55,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="56" ht="15">
       <c r="C56" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B56,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A56,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="57" ht="15">
       <c r="C57" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B57,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A57,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="58" ht="15">
       <c r="C58" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B58,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A58,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="59" ht="15">
       <c r="C59" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B59,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A59,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="60" ht="15">
       <c r="C60" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B60,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A60,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="61" ht="15">
       <c r="C61" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B61,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A61,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="62" ht="15">
       <c r="C62" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B62,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A62,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="63" ht="15">
       <c r="C63" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B63,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A63,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="64" ht="15">
       <c r="C64" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B64,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A64,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="65" ht="15">
       <c r="C65" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B65,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A65,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="66" ht="15">
       <c r="C66" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B66,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A66,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="67" ht="15">
       <c r="C67" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B67,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A67,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="68" ht="15">
       <c r="C68" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B68,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A68,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="69" ht="15">
       <c r="C69" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B69,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A69,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="70" ht="15">
       <c r="C70" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B70,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A70,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="71" ht="15">
       <c r="C71" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B71,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A71,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="72" ht="15">
       <c r="C72" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B72,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A72,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="73" ht="15">
       <c r="C73" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B73,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A73,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="74" ht="15">
       <c r="C74" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B74,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A74,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="75" ht="15">
       <c r="C75" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B75,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A75,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="76" ht="15">
       <c r="C76" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B76,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A76,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="77" ht="15">
       <c r="C77" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B77,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A77,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="78" ht="15">
       <c r="C78" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B78,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A78,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="79" ht="15">
       <c r="C79" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B79,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A79,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="80" ht="15">
       <c r="C80" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B80,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A80,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="81" ht="15">
       <c r="C81" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B81,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A81,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="82" ht="15">
       <c r="C82" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B82,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A82,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="83" ht="15">
       <c r="C83" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B83,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A83,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="84" ht="15">
       <c r="C84" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B84,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A84,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="85" ht="15">
       <c r="C85" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B85,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A85,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="86" ht="15">
       <c r="C86" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B86,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A86,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="87" ht="15">
       <c r="C87" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B87,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A87,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="88" ht="15">
       <c r="C88" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B88,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A88,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="89" ht="15">
       <c r="C89" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B89,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A89,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="90" ht="15">
       <c r="C90" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B90,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A90,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="91" ht="15">
       <c r="C91" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B91,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A91,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="92" ht="15">
       <c r="C92" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B92,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A92,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="93" ht="15">
       <c r="C93" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B93,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A93,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="94" ht="15">
       <c r="C94" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B94,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A94,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="95" ht="15">
       <c r="C95" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B95,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A95,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="96" ht="15">
       <c r="C96" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B96,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A96,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="97" ht="15">
       <c r="C97" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B97,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A97,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="98" ht="15">
       <c r="C98" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B98,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A98,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="99" ht="15">
       <c r="C99" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B99,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A99,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="100" ht="15">
       <c r="C100" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B100,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A100,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="101" ht="15">
       <c r="C101" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B101,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A101,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="102" ht="15">
       <c r="C102" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B102,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A102,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="103" ht="15">
       <c r="C103" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B103,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A103,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="104" ht="15">
       <c r="C104" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B104,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A104,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="105" ht="15">
       <c r="C105" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B105,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A105,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="106" ht="15">
       <c r="C106" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B106,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A106,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="107" ht="15">
       <c r="C107" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B107,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A107,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="108" ht="15">
       <c r="C108" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B108,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A108,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="109" ht="15">
       <c r="C109" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B109,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A109,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="110" ht="15">
       <c r="C110" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B110,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A110,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="111" ht="15">
       <c r="C111" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B111,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A111,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="112" ht="15">
       <c r="C112" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B112,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A112,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="113" ht="15">
       <c r="C113" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B113,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A113,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="114" ht="15">
       <c r="C114" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B114,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A114,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="115" ht="15">
       <c r="C115" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B115,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A115,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="116" ht="15">
       <c r="C116" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B116,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A116,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="117" ht="15">
       <c r="C117" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B117,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A117,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="118" ht="15">
       <c r="C118" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B118,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A118,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="119" ht="15">
       <c r="C119" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B119,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A119,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="120" ht="15">
       <c r="C120" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B120,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A120,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="121" ht="15">
       <c r="C121" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B121,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A121,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="122" ht="15">
       <c r="C122" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B122,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A122,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="123" ht="15">
       <c r="C123" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B123,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A123,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="124" ht="15">
       <c r="C124" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B124,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A124,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="125" ht="15">
       <c r="C125" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B125,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A125,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="126" ht="15">
       <c r="C126" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B126,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A126,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="127" ht="15">
       <c r="C127" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B127,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A127,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="128" ht="15">
       <c r="C128" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B128,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A128,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="129" ht="15">
       <c r="C129" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B129,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A129,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="130" ht="15">
       <c r="C130" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B130,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A130,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="131" ht="15">
       <c r="C131" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B131,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A131,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="132" ht="15">
       <c r="C132" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B132,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A132,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="133" ht="15">
       <c r="C133" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B133,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A133,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="134" ht="15">
       <c r="C134" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B134,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A134,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="135" ht="15">
       <c r="C135" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B135,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A135,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="136" ht="15">
       <c r="C136" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B136,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A136,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="137" ht="15">
       <c r="C137" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B137,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A137,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="138" ht="15">
       <c r="C138" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B138,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A138,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="139" ht="15">
       <c r="C139" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B139,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A139,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="140" ht="15">
       <c r="C140" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B140,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A140,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="141" ht="15">
       <c r="C141" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B141,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A141,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="142" ht="15">
       <c r="C142" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B142,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A142,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="143" ht="15">
       <c r="C143" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B143,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A143,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="144" ht="15">
       <c r="C144" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B144,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A144,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="145" ht="15">
       <c r="C145" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B145,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A145,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="146" ht="15">
       <c r="C146" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B146,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A146,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="147" ht="15">
       <c r="C147" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B147,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A147,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="148" ht="15">
       <c r="C148" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B148,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A148,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="149" ht="15">
       <c r="C149" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B149,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A149,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="150" ht="15">
       <c r="C150" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B150,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A150,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="151" ht="15">
       <c r="C151" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B151,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A151,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="152" ht="15">
       <c r="C152" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B152,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A152,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="153" ht="15">
       <c r="C153" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B153,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A153,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="154" ht="15">
       <c r="C154" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B154,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A154,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="155" ht="15">
       <c r="C155" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B155,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A155,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="156" ht="15">
       <c r="C156" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B156,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A156,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="157" ht="15">
       <c r="C157" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B157,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A157,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="158" ht="15">
       <c r="C158" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B158,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A158,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="159" ht="15">
       <c r="C159" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B159,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A159,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="160" ht="15">
       <c r="C160" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B160,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A160,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="161" ht="15">
       <c r="C161" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B161,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A161,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="162" ht="15">
       <c r="C162" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B162,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A162,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="163" ht="15">
       <c r="C163" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B163,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A163,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="164" ht="15">
       <c r="C164" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B164,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A164,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="165" ht="15">
       <c r="C165" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B165,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A165,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="166" ht="15">
       <c r="C166" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B166,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A166,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="167" ht="15">
       <c r="C167" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B167,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A167,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="168" ht="15">
       <c r="C168" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B168,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A168,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="169" ht="15">
       <c r="C169" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B169,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A169,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="170" ht="15">
       <c r="C170" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B170,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A170,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="171" ht="15">
       <c r="C171" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B171,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A171,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="172" ht="15">
       <c r="C172" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B172,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A172,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="173" ht="15">
       <c r="C173" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B173,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A173,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="174" ht="15">
       <c r="C174" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B174,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A174,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="175" ht="15">
       <c r="C175" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B175,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A175,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="176" ht="15">
       <c r="C176" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B176,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A176,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="177" ht="15">
       <c r="C177" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B177,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A177,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="178" ht="15">
       <c r="C178" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B178,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A178,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="179" ht="15">
       <c r="C179" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B179,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A179,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="180" ht="15">
       <c r="C180" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B180,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A180,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="181" ht="15">
       <c r="C181" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B181,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A181,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="182" ht="15">
       <c r="C182" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B182,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A182,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="183" ht="15">
       <c r="C183" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B183,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A183,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="184" ht="15">
       <c r="C184" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B184,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A184,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="185" ht="15">
       <c r="C185" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B185,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A185,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="186" ht="15">
       <c r="C186" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B186,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A186,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="187" ht="15">
       <c r="C187" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B187,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A187,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="188" ht="15">
       <c r="C188" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B188,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A188,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="189" ht="15">
       <c r="C189" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B189,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A189,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="190" ht="15">
       <c r="C190" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B190,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A190,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="191" ht="15">
       <c r="C191" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B191,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A191,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="192" ht="15">
       <c r="C192" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B192,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A192,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="193" ht="15">
       <c r="C193" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B193,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A193,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="194" ht="15">
       <c r="C194" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B194,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A194,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="195" ht="15">
       <c r="C195" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B195,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A195,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="196" ht="15">
       <c r="C196" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B196,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A196,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="197" ht="15">
       <c r="C197" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B197,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A197,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="198" ht="15">
       <c r="C198" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B198,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A198,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="199" ht="15">
       <c r="C199" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B199,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A199,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="200" ht="15">
       <c r="C200" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B200,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A200,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="201" ht="15">
       <c r="C201" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B201,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A201,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="202" ht="15">
       <c r="C202" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B202,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A202,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="203" ht="15">
       <c r="C203" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B203,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A203,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="204" ht="15">
       <c r="C204" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B204,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A204,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="205" ht="15">
       <c r="C205" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B205,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A205,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="206" ht="15">
       <c r="C206" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B206,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A206,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="207" ht="15">
       <c r="C207" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B207,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A207,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="208" ht="15">
       <c r="C208" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B208,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A208,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="209" ht="15">
       <c r="C209" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B209,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A209,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="210" ht="15">
       <c r="C210" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B210,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A210,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="211" ht="15">
       <c r="C211" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B211,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A211,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="212" ht="15">
       <c r="C212" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B212,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A212,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="213" ht="15">
       <c r="C213" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B213,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A213,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="214" ht="15">
       <c r="C214" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B214,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A214,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="215" ht="15">
       <c r="C215" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B215,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A215,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="216" ht="15">
       <c r="C216" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B216,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A216,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="217" ht="15">
       <c r="C217" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B217,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A217,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="218" ht="15">
       <c r="C218" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B218,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A218,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="219" ht="15">
       <c r="C219" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B219,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A219,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="220" ht="15">
       <c r="C220" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B220,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A220,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="221" ht="15">
       <c r="C221" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B221,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A221,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="222" ht="15">
       <c r="C222" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B222,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A222,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="223" ht="15">
       <c r="C223" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B223,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A223,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="224" ht="15">
       <c r="C224" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B224,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A224,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="225" ht="15">
       <c r="C225" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B225,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A225,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="226" ht="15">
       <c r="C226" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B226,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A226,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="227" ht="15">
       <c r="C227" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B227,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A227,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="228" ht="15">
       <c r="C228" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B228,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A228,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="229" ht="15">
       <c r="C229" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B229,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A229,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="230" ht="15">
       <c r="C230" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B230,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A230,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="231" ht="15">
       <c r="C231" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B231,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A231,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="232" ht="15">
       <c r="C232" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B232,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A232,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="233" ht="15">
       <c r="C233" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B233,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A233,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="234" ht="15">
       <c r="C234" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B234,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A234,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="235" ht="15">
       <c r="C235" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B235,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A235,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="236" ht="15">
       <c r="C236" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B236,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A236,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="237" ht="15">
       <c r="C237" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B237,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A237,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="238" ht="15">
       <c r="C238" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B238,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A238,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="239" ht="15">
       <c r="C239" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B239,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A239,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="240" ht="15">
       <c r="C240" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B240,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A240,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="241" ht="15">
       <c r="C241" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B241,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A241,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="242" ht="15">
       <c r="C242" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B242,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A242,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="243" ht="15">
       <c r="C243" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B243,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A243,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="244" ht="15">
       <c r="C244" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B244,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A244,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="245" ht="15">
       <c r="C245" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B245,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A245,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="246" ht="15">
       <c r="C246" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B246,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A246,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="247" ht="15">
       <c r="C247" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B247,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A247,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="248" ht="15">
       <c r="C248" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B248,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A248,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="249" ht="15">
       <c r="C249" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B249,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A249,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="250" ht="15">
       <c r="C250" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B250,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A250,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="251" ht="15">
       <c r="C251" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B251,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A251,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="252" ht="15">
       <c r="C252" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B252,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A252,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="253" ht="15">
       <c r="C253" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B253,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A253,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="254" ht="15">
       <c r="C254" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B254,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A254,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="255" ht="15">
       <c r="C255" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B255,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A255,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="256" ht="15">
       <c r="C256" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B256,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A256,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="257" ht="15">
       <c r="C257" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B257,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A257,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="258" ht="15">
       <c r="C258" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B258,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A258,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="259" ht="15">
       <c r="C259" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B259,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A259,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="260" ht="15">
       <c r="C260" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B260,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A260,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="261" ht="15">
       <c r="C261" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B261,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A261,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="262" ht="15">
       <c r="C262" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B262,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A262,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="263" ht="15">
       <c r="C263" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B263,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A263,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="264" ht="15">
       <c r="C264" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B264,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A264,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="265" ht="15">
       <c r="C265" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B265,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A265,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="266" ht="15">
       <c r="C266" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B266,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A266,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="267" ht="15">
       <c r="C267" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B267,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A267,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="268" ht="15">
       <c r="C268" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B268,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A268,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="269" ht="15">
       <c r="C269" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B269,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A269,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="270" ht="15">
       <c r="C270" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B270,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A270,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="271" ht="15">
       <c r="C271" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B271,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A271,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="272" ht="15">
       <c r="C272" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B272,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A272,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="273" ht="15">
       <c r="C273" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B273,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A273,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="274" ht="15">
       <c r="C274" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B274,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A274,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="275" ht="15">
       <c r="C275" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B275,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A275,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="276" ht="15">
       <c r="C276" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B276,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A276,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="277" ht="15">
       <c r="C277" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B277,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A277,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="278" ht="15">
       <c r="C278" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B278,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A278,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="279" ht="15">
       <c r="C279" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B279,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A279,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="280" ht="15">
       <c r="C280" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B280,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A280,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="281" ht="15">
       <c r="C281" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B281,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A281,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="282" ht="15">
       <c r="C282" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B282,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A282,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="283" ht="15">
       <c r="C283" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B283,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A283,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="284" ht="15">
       <c r="C284" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B284,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A284,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="285" ht="15">
       <c r="C285" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B285,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A285,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="286" ht="15">
       <c r="C286" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B286,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A286,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="287" ht="15">
       <c r="C287" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B287,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A287,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="288" ht="15">
       <c r="C288" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B288,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A288,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="289" ht="15">
       <c r="C289" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B289,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A289,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="290" ht="15">
       <c r="C290" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B290,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A290,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="291" ht="15">
       <c r="C291" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B291,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A291,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="292" ht="15">
       <c r="C292" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B292,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A292,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="293" ht="15">
       <c r="C293" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B293,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A293,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="294" ht="15">
       <c r="C294" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B294,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A294,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="295" ht="15">
       <c r="C295" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B295,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A295,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="296" ht="15">
       <c r="C296" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B296,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A296,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="297" ht="15">
       <c r="C297" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B297,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A297,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="298" ht="15">
       <c r="C298" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B298,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A298,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="299" ht="15">
       <c r="C299" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B299,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A299,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="300" ht="15">
       <c r="C300" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B300,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A300,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="301" ht="15">
       <c r="C301" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B301,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A301,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="302" ht="15">
       <c r="C302" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B302,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A302,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="303" ht="15">
       <c r="C303" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B303,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A303,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="304" ht="15">
       <c r="C304" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B304,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A304,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="305" ht="15">
       <c r="C305" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B305,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A305,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="306" ht="15">
       <c r="C306" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B306,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A306,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="307" ht="15">
       <c r="C307" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B307,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A307,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="308" ht="15">
       <c r="C308" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B308,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A308,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="309" ht="15">
       <c r="C309" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B309,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A309,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="310" ht="15">
       <c r="C310" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B310,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A310,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="311" ht="15">
       <c r="C311" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B311,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A311,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="312" ht="15">
       <c r="C312" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B312,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A312,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="313" ht="15">
       <c r="C313" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B313,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A313,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="314" ht="15">
       <c r="C314" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B314,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A314,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="315" ht="15">
       <c r="C315" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B315,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A315,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="316" ht="15">
       <c r="C316" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B316,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A316,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="317" ht="15">
       <c r="C317" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B317,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A317,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="318" ht="15">
       <c r="C318" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B318,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A318,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="319" ht="15">
       <c r="C319" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B319,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A319,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="320" ht="15">
       <c r="C320" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B320,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A320,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="321" ht="15">
       <c r="C321" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B321,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A321,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="322" ht="15">
       <c r="C322" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B322,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A322,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="323" ht="15">
       <c r="C323" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B323,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A323,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="324" ht="15">
       <c r="C324" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B324,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A324,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="325" ht="15">
       <c r="C325" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B325,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A325,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="326" ht="15">
       <c r="C326" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B326,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A326,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="327" ht="15">
       <c r="C327" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B327,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A327,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="328" ht="15">
       <c r="C328" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B328,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A328,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="329" ht="15">
       <c r="C329" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B329,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A329,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="330" ht="15">
       <c r="C330" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B330,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A330,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="331" ht="15">
       <c r="C331" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B331,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A331,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="332" ht="15">
       <c r="C332" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B332,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A332,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="333" ht="15">
       <c r="C333" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B333,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A333,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="334" ht="15">
       <c r="C334" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B334,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A334,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="335" ht="15">
       <c r="C335" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B335,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A335,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="336" ht="15">
       <c r="C336" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B336,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A336,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="337" ht="15">
       <c r="C337" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B337,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A337,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="338" ht="15">
       <c r="C338" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B338,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A338,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="339" ht="15">
       <c r="C339" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B339,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A339,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="340" ht="15">
       <c r="C340" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B340,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A340,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="341" ht="15">
       <c r="C341" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B341,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A341,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="342" ht="15">
       <c r="C342" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B342,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A342,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="343" ht="15">
       <c r="C343" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B343,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A343,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="344" ht="15">
       <c r="C344" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B344,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A344,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="345" ht="15">
       <c r="C345" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B345,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A345,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="346" ht="15">
       <c r="C346" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B346,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A346,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="347" ht="15">
       <c r="C347" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B347,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A347,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="348" ht="15">
       <c r="C348" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B348,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A348,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="349" ht="15">
       <c r="C349" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B349,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A349,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="350" ht="15">
       <c r="C350" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B350,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A350,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="351" ht="15">
       <c r="C351" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B351,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A351,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="352" ht="15">
       <c r="C352" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B352,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A352,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="353" ht="15">
       <c r="C353" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B353,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A353,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="354" ht="15">
       <c r="C354" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B354,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A354,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="355" ht="15">
       <c r="C355" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B355,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A355,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="356" ht="15">
       <c r="C356" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B356,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A356,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="357" ht="15">
       <c r="C357" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B357,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A357,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="358" ht="15">
       <c r="C358" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B358,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A358,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="359" ht="15">
       <c r="C359" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B359,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A359,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="360" ht="15">
       <c r="C360" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B360,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A360,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="361" ht="15">
       <c r="C361" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B361,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A361,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="362" ht="15">
       <c r="C362" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B362,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A362,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="363" ht="15">
       <c r="C363" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B363,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A363,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="364" ht="15">
       <c r="C364" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B364,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A364,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="365" ht="15">
       <c r="C365" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B365,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A365,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="366" ht="15">
       <c r="C366" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B366,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A366,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="367" ht="15">
       <c r="C367" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B367,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A367,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="368" ht="15">
       <c r="C368" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B368,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A368,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="369" ht="15">
       <c r="C369" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B369,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A369,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="370" ht="15">
       <c r="C370" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B370,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A370,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="371" ht="15">
       <c r="C371" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B371,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A371,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="372" ht="15">
       <c r="C372" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B372,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A372,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="373" ht="15">
       <c r="C373" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B373,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A373,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="374" ht="15">
       <c r="C374" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B374,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A374,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="375" ht="15">
       <c r="C375" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B375,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A375,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="376" ht="15">
       <c r="C376" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B376,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A376,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="377" ht="15">
       <c r="C377" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B377,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A377,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="378" ht="15">
       <c r="C378" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B378,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A378,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="379" ht="15">
       <c r="C379" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B379,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A379,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="380" ht="15">
       <c r="C380" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B380,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A380,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="381" ht="15">
       <c r="C381" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B381,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A381,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="382" ht="15">
       <c r="C382" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B382,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A382,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="383" ht="15">
       <c r="C383" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B383,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A383,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="384" ht="15">
       <c r="C384" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B384,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A384,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="385" ht="15">
       <c r="C385" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B385,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A385,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="386" ht="15">
       <c r="C386" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B386,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A386,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="387" ht="15">
       <c r="C387" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B387,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A387,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="388" ht="15">
       <c r="C388" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B388,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A388,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="389" ht="15">
       <c r="C389" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B389,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A389,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="390" ht="15">
       <c r="C390" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B390,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A390,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="391" ht="15">
       <c r="C391" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B391,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A391,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="392" ht="15">
       <c r="C392" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B392,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A392,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="393" ht="15">
       <c r="C393" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B393,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A393,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="394" ht="15">
       <c r="C394" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B394,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A394,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="395" ht="15">
       <c r="C395" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B395,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A395,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="396" ht="15">
       <c r="C396" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B396,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A396,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="397" ht="15">
       <c r="C397" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B397,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A397,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="398" ht="15">
       <c r="C398" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B398,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A398,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="399" ht="15">
       <c r="C399" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B399,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A399,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="400" ht="15">
       <c r="C400" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B400,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A400,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="401" ht="15">
       <c r="C401" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B401,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A401,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="402" ht="15">
       <c r="C402" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B402,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A402,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="403" ht="15">
       <c r="C403" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B403,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A403,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="404" ht="15">
       <c r="C404" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B404,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A404,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="405" ht="15">
       <c r="C405" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B405,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A405,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="406" ht="15">
       <c r="C406" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B406,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A406,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="407" ht="15">
       <c r="C407" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B407,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A407,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="408" ht="15">
       <c r="C408" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B408,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A408,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="409" ht="15">
       <c r="C409" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B409,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A409,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="410" ht="15">
       <c r="C410" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B410,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A410,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="411" ht="15">
       <c r="C411" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B411,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A411,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="412" ht="15">
       <c r="C412" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B412,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A412,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="413" ht="15">
       <c r="C413" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B413,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A413,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="414" ht="15">
       <c r="C414" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B414,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A414,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="415" ht="15">
       <c r="C415" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B415,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A415,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="416" ht="15">
       <c r="C416" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B416,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A416,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="417" ht="15">
       <c r="C417" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B417,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A417,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="418" ht="15">
       <c r="C418" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B418,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A418,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="419" ht="15">
       <c r="C419" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B419,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A419,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="420" ht="15">
       <c r="C420" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B420,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A420,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="421" ht="15">
       <c r="C421" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B421,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A421,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="422" ht="15">
       <c r="C422" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B422,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A422,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="423" ht="15">
       <c r="C423" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B423,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A423,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="424" ht="15">
       <c r="C424" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B424,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A424,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="425" ht="15">
       <c r="C425" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B425,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A425,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="426" ht="15">
       <c r="C426" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B426,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A426,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="427" ht="15">
       <c r="C427" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B427,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A427,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="428" ht="15">
       <c r="C428" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B428,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A428,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="429" ht="15">
       <c r="C429" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B429,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A429,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="430" ht="15">
       <c r="C430" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B430,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A430,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="431" ht="15">
       <c r="C431" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B431,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A431,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="432" ht="15">
       <c r="C432" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B432,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A432,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="433" ht="15">
       <c r="C433" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B433,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A433,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="434" ht="15">
       <c r="C434" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B434,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A434,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="435" ht="15">
       <c r="C435" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B435,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A435,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="436" ht="15">
       <c r="C436" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B436,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A436,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="437" ht="15">
       <c r="C437" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B437,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A437,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="438" ht="15">
       <c r="C438" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B438,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A438,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="439" ht="15">
       <c r="C439" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B439,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A439,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="440" ht="15">
       <c r="C440" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B440,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A440,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="441" ht="15">
       <c r="C441" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B441,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A441,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="442" ht="15">
       <c r="C442" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B442,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A442,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="443" ht="15">
       <c r="C443" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B443,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A443,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="444" ht="15">
       <c r="C444" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B444,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A444,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="445" ht="15">
       <c r="C445" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B445,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A445,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="446" ht="15">
       <c r="C446" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B446,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A446,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="447" ht="15">
       <c r="C447" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B447,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A447,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="448" ht="15">
       <c r="C448" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B448,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A448,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="449" ht="15">
       <c r="C449" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B449,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A449,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="450" ht="15">
       <c r="C450" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B450,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A450,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="451" ht="15">
       <c r="C451" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B451,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A451,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="452" ht="15">
       <c r="C452" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B452,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A452,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="453" ht="15">
       <c r="C453" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B453,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A453,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="454" ht="15">
       <c r="C454" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B454,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A454,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="455" ht="15">
       <c r="C455" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B455,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A455,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="456" ht="15">
       <c r="C456" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B456,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A456,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="457" ht="15">
       <c r="C457" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B457,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A457,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="458" ht="15">
       <c r="C458" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B458,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A458,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="459" ht="15">
       <c r="C459" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B459,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A459,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="460" ht="15">
       <c r="C460" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B460,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A460,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="461" ht="15">
       <c r="C461" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B461,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A461,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="462" ht="15">
       <c r="C462" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B462,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A462,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="463" ht="15">
       <c r="C463" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B463,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A463,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="464" ht="15">
       <c r="C464" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B464,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A464,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="465" ht="15">
       <c r="C465" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B465,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A465,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="466" ht="15">
       <c r="C466" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B466,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A466,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="467" ht="15">
       <c r="C467" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B467,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A467,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="468" ht="15">
       <c r="C468" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B468,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A468,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="469" ht="15">
       <c r="C469" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B469,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A469,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="470" ht="15">
       <c r="C470" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B470,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A470,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="471" ht="15">
       <c r="C471" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B471,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A471,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="472" ht="15">
       <c r="C472" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B472,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A472,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="473" ht="15">
       <c r="C473" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B473,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A473,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="474" ht="15">
       <c r="C474" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B474,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A474,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="475" ht="15">
       <c r="C475" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B475,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A475,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="476" ht="15">
       <c r="C476" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B476,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A476,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="477" ht="15">
       <c r="C477" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B477,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A477,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="478" ht="15">
       <c r="C478" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B478,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A478,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="479" ht="15">
       <c r="C479" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B479,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A479,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="480" ht="15">
       <c r="C480" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B480,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A480,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="481" ht="15">
       <c r="C481" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B481,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A481,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="482" ht="15">
       <c r="C482" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B482,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A482,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="483" ht="15">
       <c r="C483" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B483,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A483,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="484" ht="15">
       <c r="C484" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B484,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A484,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="485" ht="15">
       <c r="C485" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B485,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A485,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="486" ht="15">
       <c r="C486" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B486,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A486,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="487" ht="15">
       <c r="C487" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B487,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A487,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="488" ht="15">
       <c r="C488" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B488,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A488,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="489" ht="15">
       <c r="C489" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B489,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A489,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="490" ht="15">
       <c r="C490" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B490,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A490,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="491" ht="15">
       <c r="C491" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B491,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A491,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="492" ht="15">
       <c r="C492" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B492,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A492,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="493" ht="15">
       <c r="C493" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B493,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A493,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="494" ht="15">
       <c r="C494" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B494,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A494,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="495" ht="15">
       <c r="C495" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B495,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A495,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="496" ht="15">
       <c r="C496" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B496,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A496,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="497" ht="15">
       <c r="C497" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B497,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A497,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="498" ht="15">
       <c r="C498" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B498,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A498,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="499" ht="15">
       <c r="C499" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B499,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A499,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="500" ht="15">
       <c r="C500" s="8" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH($B500,OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
+        <f ca="1">IFERROR(INDEX(OFFSET('[1]Sheet1'!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET('[2]Sheet1'!$B$1,0,0,MaxCount),MATCH($A500,OFFSET('[2]Sheet1'!$A$1,0,0,MaxCount),0),1),OFFSET('[1]Sheet1'!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
feat:update bag dragon icon change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Dragon_龙表.xlsx
+++ b/dragon-verse/Excels/Dragon_龙表.xlsx
@@ -375,12 +375,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,15 +392,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,19 +408,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -665,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:M2000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -686,7 +674,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -698,7 +686,7 @@
       <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -727,7 +715,7 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -739,7 +727,7 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -768,13 +756,13 @@
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -802,37 +790,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="9"/>
-      <c r="E4" s="10"/>
+    <row r="4" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="11" t="str">
+      <c r="C5" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D5,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J5" s="1" t="n">
@@ -846,32 +833,32 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="11" t="str">
+      <c r="C6" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D6,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="n">
@@ -885,32 +872,32 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="11" t="str">
+      <c r="C7" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D7,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J7" s="1" t="n">
@@ -924,32 +911,32 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="11" t="str">
+      <c r="C8" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D8,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J8" s="1" t="n">
@@ -963,32 +950,32 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="11" t="str">
+      <c r="C9" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D9,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J9" s="1" t="n">
@@ -1002,32 +989,32 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="11" t="str">
+      <c r="C10" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D10,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J10" s="1" t="n">
@@ -1041,32 +1028,32 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="11" t="str">
+      <c r="C11" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D11,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J11" s="1" t="n">
@@ -1080,32 +1067,32 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="11" t="str">
+      <c r="C12" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D12,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J12" s="1" t="n">
@@ -1119,32 +1106,32 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="11" t="str">
+      <c r="C13" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D13,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J13" s="1" t="n">
@@ -1158,32 +1145,32 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="11" t="str">
+      <c r="C14" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D14,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J14" s="1" t="n">
@@ -1197,32 +1184,32 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="11" t="str">
+      <c r="C15" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D15,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J15" s="1" t="n">
@@ -1236,32 +1223,32 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="11" t="str">
+      <c r="C16" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D16,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J16" s="1" t="n">
@@ -1275,32 +1262,32 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="11" t="str">
+      <c r="C17" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D17,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G17" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J17" s="1" t="n">
@@ -1314,32 +1301,32 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="11" t="str">
+      <c r="C18" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D18,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J18" s="1" t="n">
@@ -1353,32 +1340,32 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="11" t="str">
+      <c r="C19" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D19,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J19" s="1" t="n">
@@ -1392,32 +1379,32 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="11" t="str">
+      <c r="C20" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D20,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J20" s="1" t="n">
@@ -1431,32 +1418,32 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="11" t="str">
+      <c r="C21" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D21,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J21" s="1" t="n">
@@ -1470,32 +1457,32 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="11" t="str">
+      <c r="C22" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D22,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J22" s="1" t="n">
@@ -1509,32 +1496,32 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="11" t="str">
+      <c r="C23" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D23,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J23" s="1" t="n">
@@ -1548,32 +1535,32 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="11" t="str">
+      <c r="C24" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D24,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J24" s="1" t="n">
@@ -1587,32 +1574,32 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="11" t="str">
+      <c r="C25" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D25,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J25" s="1" t="n">
@@ -1626,32 +1613,32 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="11" t="str">
+      <c r="C26" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D26,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J26" s="1" t="n">
@@ -1665,32 +1652,32 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="11" t="str">
+      <c r="C27" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D27,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="I27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J27" s="1" t="n">
@@ -1704,32 +1691,32 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="11" t="str">
+      <c r="C28" s="8" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D28,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="I28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J28" s="1" t="n">
@@ -1743,32 +1730,32 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="9" t="str">
+      <c r="C29" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D29,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I29" s="0" t="n">
+      <c r="I29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J29" s="1" t="n">
@@ -1782,32 +1769,32 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="9" t="str">
+      <c r="C30" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D30,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="I30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J30" s="1" t="n">
@@ -1821,32 +1808,32 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="9" t="str">
+      <c r="C31" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D31,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I31" s="0" t="n">
+      <c r="I31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J31" s="1" t="n">
@@ -1860,32 +1847,32 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="9" t="str">
+      <c r="C32" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D32,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="0" t="n">
+      <c r="I32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J32" s="1" t="n">
@@ -1899,32 +1886,32 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="9" t="str">
+      <c r="C33" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D33,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I33" s="0" t="n">
+      <c r="I33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J33" s="1" t="n">
@@ -1938,32 +1925,32 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="9" t="str">
+      <c r="C34" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D34,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I34" s="0" t="n">
+      <c r="I34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J34" s="1" t="n">
@@ -1977,32 +1964,32 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="9" t="str">
+      <c r="C35" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D35,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I35" s="0" t="n">
+      <c r="I35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J35" s="1" t="n">
@@ -2016,32 +2003,32 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="9" t="str">
+      <c r="C36" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D36,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="0" t="n">
+      <c r="I36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J36" s="1" t="n">
@@ -2055,32 +2042,32 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="9" t="str">
+      <c r="C37" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D37,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I37" s="0" t="n">
+      <c r="I37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J37" s="1" t="n">
@@ -2094,32 +2081,32 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="9" t="str">
+      <c r="C38" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D38,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I38" s="0" t="n">
+      <c r="I38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J38" s="1" t="n">
@@ -2133,32 +2120,32 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="9" t="str">
+      <c r="C39" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D39,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I39" s="0" t="n">
+      <c r="I39" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J39" s="1" t="n">
@@ -2172,32 +2159,32 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="9" t="str">
+      <c r="C40" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D40,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="H40" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I40" s="0" t="n">
+      <c r="I40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J40" s="1" t="n">
@@ -2211,32 +2198,32 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="9" t="str">
+      <c r="C41" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D41,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I41" s="0" t="n">
+      <c r="I41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J41" s="1" t="n">
@@ -2250,32 +2237,32 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="9" t="str">
+      <c r="C42" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D42,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I42" s="0" t="n">
+      <c r="I42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J42" s="1" t="n">
@@ -2289,32 +2276,32 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="9" t="str">
+      <c r="C43" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D43,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="F43" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="H43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I43" s="0" t="n">
+      <c r="I43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J43" s="1" t="n">
@@ -2328,32 +2315,32 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="9" t="str">
+      <c r="C44" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D44,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F44" s="0" t="n">
+      <c r="F44" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="H44" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I44" s="0" t="n">
+      <c r="I44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J44" s="1" t="n">
@@ -2367,32 +2354,32 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="9" t="str">
+      <c r="C45" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D45,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="E45" s="0" t="n">
+      <c r="E45" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="F45" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="H45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I45" s="0" t="n">
+      <c r="I45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J45" s="1" t="n">
@@ -2406,32 +2393,32 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="9" t="str">
+      <c r="C46" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D46,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46" s="1" t="n">
         <v>3</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="H46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I46" s="0" t="n">
+      <c r="I46" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J46" s="1" t="n">
@@ -2445,2725 +2432,2725 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="9" t="str">
+      <c r="C47" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D47,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="9" t="str">
+      <c r="C48" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D48,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="9" t="str">
+      <c r="C49" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D49,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="9" t="str">
+      <c r="C50" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D50,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="9" t="str">
+      <c r="C51" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D51,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="9" t="str">
+      <c r="C52" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D52,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="9" t="str">
+      <c r="C53" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D53,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="9" t="str">
+      <c r="C54" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D54,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="9" t="str">
+      <c r="C55" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D55,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="9" t="str">
+      <c r="C56" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D56,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="9" t="str">
+      <c r="C57" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D57,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="9" t="str">
+      <c r="C58" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D58,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="9" t="str">
+      <c r="C59" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D59,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="9" t="str">
+      <c r="C60" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D60,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="9" t="str">
+      <c r="C61" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D61,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="9" t="str">
+      <c r="C62" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D62,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="9" t="str">
+      <c r="C63" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D63,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="9" t="str">
+      <c r="C64" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D64,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="9" t="str">
+      <c r="C65" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D65,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="9" t="str">
+      <c r="C66" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D66,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="9" t="str">
+      <c r="C67" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D67,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="9" t="str">
+      <c r="C68" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D68,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="9" t="str">
+      <c r="C69" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D69,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="9" t="str">
+      <c r="C70" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D70,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="9" t="str">
+      <c r="C71" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D71,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="9" t="str">
+      <c r="C72" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D72,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="9" t="str">
+      <c r="C73" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D73,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="9" t="str">
+      <c r="C74" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D74,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C75" s="9" t="str">
+      <c r="C75" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D75,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="9" t="str">
+      <c r="C76" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D76,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="9" t="str">
+      <c r="C77" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D77,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="9" t="str">
+      <c r="C78" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D78,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="9" t="str">
+      <c r="C79" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D79,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="9" t="str">
+      <c r="C80" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D80,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C81" s="9" t="str">
+      <c r="C81" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D81,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="9" t="str">
+      <c r="C82" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D82,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="9" t="str">
+      <c r="C83" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D83,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="9" t="str">
+      <c r="C84" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D84,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="9" t="str">
+      <c r="C85" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D85,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="9" t="str">
+      <c r="C86" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D86,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="9" t="str">
+      <c r="C87" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D87,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="9" t="str">
+      <c r="C88" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D88,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="9" t="str">
+      <c r="C89" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D89,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="9" t="str">
+      <c r="C90" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D90,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="9" t="str">
+      <c r="C91" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D91,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="9" t="str">
+      <c r="C92" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D92,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="9" t="str">
+      <c r="C93" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D93,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="9" t="str">
+      <c r="C94" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D94,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="9" t="str">
+      <c r="C95" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D95,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C96" s="9" t="str">
+      <c r="C96" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D96,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="9" t="str">
+      <c r="C97" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D97,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="9" t="str">
+      <c r="C98" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D98,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="9" t="str">
+      <c r="C99" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D99,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C100" s="9" t="str">
+      <c r="C100" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D100,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="9" t="str">
+      <c r="C101" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D101,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="9" t="str">
+      <c r="C102" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D102,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="9" t="str">
+      <c r="C103" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D103,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="9" t="str">
+      <c r="C104" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D104,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="9" t="str">
+      <c r="C105" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D105,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C106" s="9" t="str">
+      <c r="C106" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D106,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="9" t="str">
+      <c r="C107" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D107,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="9" t="str">
+      <c r="C108" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D108,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C109" s="9" t="str">
+      <c r="C109" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D109,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="9" t="str">
+      <c r="C110" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D110,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="9" t="str">
+      <c r="C111" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D111,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="9" t="str">
+      <c r="C112" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D112,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C113" s="9" t="str">
+      <c r="C113" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D113,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="9" t="str">
+      <c r="C114" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D114,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="9" t="str">
+      <c r="C115" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D115,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="9" t="str">
+      <c r="C116" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D116,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="9" t="str">
+      <c r="C117" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D117,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="9" t="str">
+      <c r="C118" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D118,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="9" t="str">
+      <c r="C119" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D119,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="9" t="str">
+      <c r="C120" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D120,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="9" t="str">
+      <c r="C121" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D121,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="9" t="str">
+      <c r="C122" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D122,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C123" s="9" t="str">
+      <c r="C123" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D123,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C124" s="9" t="str">
+      <c r="C124" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D124,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C125" s="9" t="str">
+      <c r="C125" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D125,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="9" t="str">
+      <c r="C126" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D126,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="9" t="str">
+      <c r="C127" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D127,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="9" t="str">
+      <c r="C128" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D128,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C129" s="9" t="str">
+      <c r="C129" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D129,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C130" s="9" t="str">
+      <c r="C130" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D130,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="9" t="str">
+      <c r="C131" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D131,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="9" t="str">
+      <c r="C132" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D132,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C133" s="9" t="str">
+      <c r="C133" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D133,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="9" t="str">
+      <c r="C134" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D134,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="9" t="str">
+      <c r="C135" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D135,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C136" s="9" t="str">
+      <c r="C136" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D136,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C137" s="9" t="str">
+      <c r="C137" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D137,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="9" t="str">
+      <c r="C138" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D138,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="9" t="str">
+      <c r="C139" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D139,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C140" s="9" t="str">
+      <c r="C140" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D140,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C141" s="9" t="str">
+      <c r="C141" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D141,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C142" s="9" t="str">
+      <c r="C142" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D142,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="9" t="str">
+      <c r="C143" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D143,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C144" s="9" t="str">
+      <c r="C144" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D144,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C145" s="9" t="str">
+      <c r="C145" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D145,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C146" s="9" t="str">
+      <c r="C146" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D146,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="9" t="str">
+      <c r="C147" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D147,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="9" t="str">
+      <c r="C148" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D148,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C149" s="9" t="str">
+      <c r="C149" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D149,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C150" s="9" t="str">
+      <c r="C150" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D150,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="9" t="str">
+      <c r="C151" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D151,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="9" t="str">
+      <c r="C152" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D152,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="9" t="str">
+      <c r="C153" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D153,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="9" t="str">
+      <c r="C154" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D154,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="9" t="str">
+      <c r="C155" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D155,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C156" s="9" t="str">
+      <c r="C156" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D156,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="9" t="str">
+      <c r="C157" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D157,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C158" s="9" t="str">
+      <c r="C158" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D158,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="9" t="str">
+      <c r="C159" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D159,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="9" t="str">
+      <c r="C160" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D160,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="9" t="str">
+      <c r="C161" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D161,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="9" t="str">
+      <c r="C162" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D162,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="9" t="str">
+      <c r="C163" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D163,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="9" t="str">
+      <c r="C164" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D164,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C165" s="9" t="str">
+      <c r="C165" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D165,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C166" s="9" t="str">
+      <c r="C166" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D166,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C167" s="9" t="str">
+      <c r="C167" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D167,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="9" t="str">
+      <c r="C168" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D168,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C169" s="9" t="str">
+      <c r="C169" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D169,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="9" t="str">
+      <c r="C170" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D170,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="9" t="str">
+      <c r="C171" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D171,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="9" t="str">
+      <c r="C172" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D172,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="9" t="str">
+      <c r="C173" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D173,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C174" s="9" t="str">
+      <c r="C174" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D174,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="9" t="str">
+      <c r="C175" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D175,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="9" t="str">
+      <c r="C176" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D176,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C177" s="9" t="str">
+      <c r="C177" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D177,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="9" t="str">
+      <c r="C178" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D178,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C179" s="9" t="str">
+      <c r="C179" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D179,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C180" s="9" t="str">
+      <c r="C180" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D180,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="9" t="str">
+      <c r="C181" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D181,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="9" t="str">
+      <c r="C182" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D182,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="9" t="str">
+      <c r="C183" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D183,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="9" t="str">
+      <c r="C184" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D184,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="9" t="str">
+      <c r="C185" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D185,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="9" t="str">
+      <c r="C186" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D186,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C187" s="9" t="str">
+      <c r="C187" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D187,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C188" s="9" t="str">
+      <c r="C188" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D188,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C189" s="9" t="str">
+      <c r="C189" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D189,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C190" s="9" t="str">
+      <c r="C190" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D190,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C191" s="9" t="str">
+      <c r="C191" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D191,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="9" t="str">
+      <c r="C192" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D192,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C193" s="9" t="str">
+      <c r="C193" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D193,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="9" t="str">
+      <c r="C194" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D194,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="9" t="str">
+      <c r="C195" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D195,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C196" s="9" t="str">
+      <c r="C196" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D196,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C197" s="9" t="str">
+      <c r="C197" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D197,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C198" s="9" t="str">
+      <c r="C198" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D198,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="9" t="str">
+      <c r="C199" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D199,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="9" t="str">
+      <c r="C200" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D200,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C201" s="9" t="str">
+      <c r="C201" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D201,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C202" s="9" t="str">
+      <c r="C202" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D202,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="9" t="str">
+      <c r="C203" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D203,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="9" t="str">
+      <c r="C204" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D204,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C205" s="9" t="str">
+      <c r="C205" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D205,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="9" t="str">
+      <c r="C206" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D206,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="9" t="str">
+      <c r="C207" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D207,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C208" s="9" t="str">
+      <c r="C208" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D208,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C209" s="9" t="str">
+      <c r="C209" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D209,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="9" t="str">
+      <c r="C210" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D210,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C211" s="9" t="str">
+      <c r="C211" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D211,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C212" s="9" t="str">
+      <c r="C212" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D212,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="9" t="str">
+      <c r="C213" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D213,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="9" t="str">
+      <c r="C214" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D214,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="9" t="str">
+      <c r="C215" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D215,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C216" s="9" t="str">
+      <c r="C216" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D216,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C217" s="9" t="str">
+      <c r="C217" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D217,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="9" t="str">
+      <c r="C218" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D218,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="9" t="str">
+      <c r="C219" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D219,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C220" s="9" t="str">
+      <c r="C220" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D220,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="9" t="str">
+      <c r="C221" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D221,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="9" t="str">
+      <c r="C222" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D222,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="9" t="str">
+      <c r="C223" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D223,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="9" t="str">
+      <c r="C224" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D224,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C225" s="9" t="str">
+      <c r="C225" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D225,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="9" t="str">
+      <c r="C226" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D226,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="9" t="str">
+      <c r="C227" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D227,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C228" s="9" t="str">
+      <c r="C228" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D228,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C229" s="9" t="str">
+      <c r="C229" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D229,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="9" t="str">
+      <c r="C230" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D230,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C231" s="9" t="str">
+      <c r="C231" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D231,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C232" s="9" t="str">
+      <c r="C232" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D232,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C233" s="9" t="str">
+      <c r="C233" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D233,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="9" t="str">
+      <c r="C234" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D234,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="9" t="str">
+      <c r="C235" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D235,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C236" s="9" t="str">
+      <c r="C236" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D236,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C237" s="9" t="str">
+      <c r="C237" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D237,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C238" s="9" t="str">
+      <c r="C238" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D238,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C239" s="9" t="str">
+      <c r="C239" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D239,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C240" s="9" t="str">
+      <c r="C240" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D240,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C241" s="9" t="str">
+      <c r="C241" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D241,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C242" s="9" t="str">
+      <c r="C242" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D242,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C243" s="9" t="str">
+      <c r="C243" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D243,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C244" s="9" t="str">
+      <c r="C244" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D244,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C245" s="9" t="str">
+      <c r="C245" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D245,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C246" s="9" t="str">
+      <c r="C246" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D246,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C247" s="9" t="str">
+      <c r="C247" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D247,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C248" s="9" t="str">
+      <c r="C248" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D248,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C249" s="9" t="str">
+      <c r="C249" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D249,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C250" s="9" t="str">
+      <c r="C250" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D250,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C251" s="9" t="str">
+      <c r="C251" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D251,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C252" s="9" t="str">
+      <c r="C252" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D252,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="9" t="str">
+      <c r="C253" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D253,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C254" s="9" t="str">
+      <c r="C254" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D254,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C255" s="9" t="str">
+      <c r="C255" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D255,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C256" s="9" t="str">
+      <c r="C256" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D256,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C257" s="9" t="str">
+      <c r="C257" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D257,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C258" s="9" t="str">
+      <c r="C258" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D258,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C259" s="9" t="str">
+      <c r="C259" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D259,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C260" s="9" t="str">
+      <c r="C260" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D260,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C261" s="9" t="str">
+      <c r="C261" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D261,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C262" s="9" t="str">
+      <c r="C262" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D262,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C263" s="9" t="str">
+      <c r="C263" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D263,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C264" s="9" t="str">
+      <c r="C264" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D264,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C265" s="9" t="str">
+      <c r="C265" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D265,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C266" s="9" t="str">
+      <c r="C266" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D266,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C267" s="9" t="str">
+      <c r="C267" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D267,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C268" s="9" t="str">
+      <c r="C268" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D268,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C269" s="9" t="str">
+      <c r="C269" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D269,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C270" s="9" t="str">
+      <c r="C270" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D270,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C271" s="9" t="str">
+      <c r="C271" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D271,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C272" s="9" t="str">
+      <c r="C272" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D272,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C273" s="9" t="str">
+      <c r="C273" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D273,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C274" s="9" t="str">
+      <c r="C274" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D274,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C275" s="9" t="str">
+      <c r="C275" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D275,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C276" s="9" t="str">
+      <c r="C276" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D276,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C277" s="9" t="str">
+      <c r="C277" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D277,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C278" s="9" t="str">
+      <c r="C278" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D278,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C279" s="9" t="str">
+      <c r="C279" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D279,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C280" s="9" t="str">
+      <c r="C280" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D280,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C281" s="9" t="str">
+      <c r="C281" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D281,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C282" s="9" t="str">
+      <c r="C282" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D282,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C283" s="9" t="str">
+      <c r="C283" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D283,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C284" s="9" t="str">
+      <c r="C284" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D284,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C285" s="9" t="str">
+      <c r="C285" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D285,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C286" s="9" t="str">
+      <c r="C286" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D286,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C287" s="9" t="str">
+      <c r="C287" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D287,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C288" s="9" t="str">
+      <c r="C288" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D288,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C289" s="9" t="str">
+      <c r="C289" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D289,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C290" s="9" t="str">
+      <c r="C290" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D290,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C291" s="9" t="str">
+      <c r="C291" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D291,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C292" s="9" t="str">
+      <c r="C292" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D292,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C293" s="9" t="str">
+      <c r="C293" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D293,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C294" s="9" t="str">
+      <c r="C294" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D294,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C295" s="9" t="str">
+      <c r="C295" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D295,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C296" s="9" t="str">
+      <c r="C296" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D296,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C297" s="9" t="str">
+      <c r="C297" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D297,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="9" t="str">
+      <c r="C298" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D298,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C299" s="9" t="str">
+      <c r="C299" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D299,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C300" s="9" t="str">
+      <c r="C300" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D300,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C301" s="9" t="str">
+      <c r="C301" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D301,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C302" s="9" t="str">
+      <c r="C302" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D302,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C303" s="9" t="str">
+      <c r="C303" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D303,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C304" s="9" t="str">
+      <c r="C304" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D304,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C305" s="9" t="str">
+      <c r="C305" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D305,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C306" s="9" t="str">
+      <c r="C306" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D306,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C307" s="9" t="str">
+      <c r="C307" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D307,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C308" s="9" t="str">
+      <c r="C308" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D308,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C309" s="9" t="str">
+      <c r="C309" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D309,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C310" s="9" t="str">
+      <c r="C310" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D310,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C311" s="9" t="str">
+      <c r="C311" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D311,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C312" s="9" t="str">
+      <c r="C312" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D312,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C313" s="9" t="str">
+      <c r="C313" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D313,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C314" s="9" t="str">
+      <c r="C314" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D314,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C315" s="9" t="str">
+      <c r="C315" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D315,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C316" s="9" t="str">
+      <c r="C316" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D316,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C317" s="9" t="str">
+      <c r="C317" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D317,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C318" s="9" t="str">
+      <c r="C318" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D318,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C319" s="9" t="str">
+      <c r="C319" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D319,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C320" s="9" t="str">
+      <c r="C320" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D320,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C321" s="9" t="str">
+      <c r="C321" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D321,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C322" s="9" t="str">
+      <c r="C322" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D322,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C323" s="9" t="str">
+      <c r="C323" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D323,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C324" s="9" t="str">
+      <c r="C324" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D324,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C325" s="9" t="str">
+      <c r="C325" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D325,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C326" s="9" t="str">
+      <c r="C326" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D326,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C327" s="9" t="str">
+      <c r="C327" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D327,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C328" s="9" t="str">
+      <c r="C328" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D328,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C329" s="9" t="str">
+      <c r="C329" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D329,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C330" s="9" t="str">
+      <c r="C330" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D330,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C331" s="9" t="str">
+      <c r="C331" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D331,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C332" s="9" t="str">
+      <c r="C332" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D332,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C333" s="9" t="str">
+      <c r="C333" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D333,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C334" s="9" t="str">
+      <c r="C334" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D334,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C335" s="9" t="str">
+      <c r="C335" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D335,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C336" s="9" t="str">
+      <c r="C336" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D336,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C337" s="9" t="str">
+      <c r="C337" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D337,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C338" s="9" t="str">
+      <c r="C338" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D338,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C339" s="9" t="str">
+      <c r="C339" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D339,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C340" s="9" t="str">
+      <c r="C340" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D340,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C341" s="9" t="str">
+      <c r="C341" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D341,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C342" s="9" t="str">
+      <c r="C342" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D342,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C343" s="9" t="str">
+      <c r="C343" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D343,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C344" s="9" t="str">
+      <c r="C344" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D344,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C345" s="9" t="str">
+      <c r="C345" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D345,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C346" s="9" t="str">
+      <c r="C346" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D346,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C347" s="9" t="str">
+      <c r="C347" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D347,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C348" s="9" t="str">
+      <c r="C348" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D348,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C349" s="9" t="str">
+      <c r="C349" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D349,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C350" s="9" t="str">
+      <c r="C350" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D350,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C351" s="9" t="str">
+      <c r="C351" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D351,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C352" s="9" t="str">
+      <c r="C352" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D352,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C353" s="9" t="str">
+      <c r="C353" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D353,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C354" s="9" t="str">
+      <c r="C354" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D354,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C355" s="9" t="str">
+      <c r="C355" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D355,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C356" s="9" t="str">
+      <c r="C356" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D356,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C357" s="9" t="str">
+      <c r="C357" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D357,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C358" s="9" t="str">
+      <c r="C358" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D358,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C359" s="9" t="str">
+      <c r="C359" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D359,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C360" s="9" t="str">
+      <c r="C360" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D360,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C361" s="9" t="str">
+      <c r="C361" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D361,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C362" s="9" t="str">
+      <c r="C362" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D362,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C363" s="9" t="str">
+      <c r="C363" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D363,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C364" s="9" t="str">
+      <c r="C364" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D364,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C365" s="9" t="str">
+      <c r="C365" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D365,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C366" s="9" t="str">
+      <c r="C366" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D366,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C367" s="9" t="str">
+      <c r="C367" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D367,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C368" s="9" t="str">
+      <c r="C368" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D368,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C369" s="9" t="str">
+      <c r="C369" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D369,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C370" s="9" t="str">
+      <c r="C370" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D370,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C371" s="9" t="str">
+      <c r="C371" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D371,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C372" s="9" t="str">
+      <c r="C372" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D372,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C373" s="9" t="str">
+      <c r="C373" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D373,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C374" s="9" t="str">
+      <c r="C374" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D374,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C375" s="9" t="str">
+      <c r="C375" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D375,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C376" s="9" t="str">
+      <c r="C376" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D376,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C377" s="9" t="str">
+      <c r="C377" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D377,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C378" s="9" t="str">
+      <c r="C378" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D378,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C379" s="9" t="str">
+      <c r="C379" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D379,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C380" s="9" t="str">
+      <c r="C380" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D380,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C381" s="9" t="str">
+      <c r="C381" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D381,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C382" s="9" t="str">
+      <c r="C382" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D382,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C383" s="9" t="str">
+      <c r="C383" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D383,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C384" s="9" t="str">
+      <c r="C384" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D384,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C385" s="9" t="str">
+      <c r="C385" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D385,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C386" s="9" t="str">
+      <c r="C386" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D386,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C387" s="9" t="str">
+      <c r="C387" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D387,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C388" s="9" t="str">
+      <c r="C388" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D388,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C389" s="9" t="str">
+      <c r="C389" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D389,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C390" s="9" t="str">
+      <c r="C390" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D390,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C391" s="9" t="str">
+      <c r="C391" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D391,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C392" s="9" t="str">
+      <c r="C392" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D392,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C393" s="9" t="str">
+      <c r="C393" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D393,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C394" s="9" t="str">
+      <c r="C394" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D394,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C395" s="9" t="str">
+      <c r="C395" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D395,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C396" s="9" t="str">
+      <c r="C396" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D396,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C397" s="9" t="str">
+      <c r="C397" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D397,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C398" s="9" t="str">
+      <c r="C398" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D398,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C399" s="9" t="str">
+      <c r="C399" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D399,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C400" s="9" t="str">
+      <c r="C400" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D400,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C401" s="9" t="str">
+      <c r="C401" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D401,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C402" s="9" t="str">
+      <c r="C402" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D402,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C403" s="9" t="str">
+      <c r="C403" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D403,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C404" s="9" t="str">
+      <c r="C404" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D404,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C405" s="9" t="str">
+      <c r="C405" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D405,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C406" s="9" t="str">
+      <c r="C406" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D406,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C407" s="9" t="str">
+      <c r="C407" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D407,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C408" s="9" t="str">
+      <c r="C408" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D408,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C409" s="9" t="str">
+      <c r="C409" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D409,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C410" s="9" t="str">
+      <c r="C410" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D410,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C411" s="9" t="str">
+      <c r="C411" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D411,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C412" s="9" t="str">
+      <c r="C412" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D412,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C413" s="9" t="str">
+      <c r="C413" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D413,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C414" s="9" t="str">
+      <c r="C414" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D414,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C415" s="9" t="str">
+      <c r="C415" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D415,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C416" s="9" t="str">
+      <c r="C416" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D416,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C417" s="9" t="str">
+      <c r="C417" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D417,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C418" s="9" t="str">
+      <c r="C418" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D418,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C419" s="9" t="str">
+      <c r="C419" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D419,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C420" s="9" t="str">
+      <c r="C420" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D420,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C421" s="9" t="str">
+      <c r="C421" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D421,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C422" s="9" t="str">
+      <c r="C422" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D422,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C423" s="9" t="str">
+      <c r="C423" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D423,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C424" s="9" t="str">
+      <c r="C424" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D424,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C425" s="9" t="str">
+      <c r="C425" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D425,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C426" s="9" t="str">
+      <c r="C426" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D426,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C427" s="9" t="str">
+      <c r="C427" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D427,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="9" t="str">
+      <c r="C428" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D428,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C429" s="9" t="str">
+      <c r="C429" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D429,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="9" t="str">
+      <c r="C430" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D430,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C431" s="9" t="str">
+      <c r="C431" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D431,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C432" s="9" t="str">
+      <c r="C432" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D432,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C433" s="9" t="str">
+      <c r="C433" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D433,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C434" s="9" t="str">
+      <c r="C434" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D434,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C435" s="9" t="str">
+      <c r="C435" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D435,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C436" s="9" t="str">
+      <c r="C436" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D436,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C437" s="9" t="str">
+      <c r="C437" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D437,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C438" s="9" t="str">
+      <c r="C438" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D438,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C439" s="9" t="str">
+      <c r="C439" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D439,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C440" s="9" t="str">
+      <c r="C440" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D440,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C441" s="9" t="str">
+      <c r="C441" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D441,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C442" s="9" t="str">
+      <c r="C442" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D442,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C443" s="9" t="str">
+      <c r="C443" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D443,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C444" s="9" t="str">
+      <c r="C444" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D444,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C445" s="9" t="str">
+      <c r="C445" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D445,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C446" s="9" t="str">
+      <c r="C446" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D446,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="447" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C447" s="9" t="str">
+      <c r="C447" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D447,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C448" s="9" t="str">
+      <c r="C448" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D448,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C449" s="9" t="str">
+      <c r="C449" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D449,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C450" s="9" t="str">
+      <c r="C450" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D450,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C451" s="9" t="str">
+      <c r="C451" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D451,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="452" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C452" s="9" t="str">
+      <c r="C452" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D452,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C453" s="9" t="str">
+      <c r="C453" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D453,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="454" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C454" s="9" t="str">
+      <c r="C454" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D454,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="455" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C455" s="9" t="str">
+      <c r="C455" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D455,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C456" s="9" t="str">
+      <c r="C456" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D456,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="457" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C457" s="9" t="str">
+      <c r="C457" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D457,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="458" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C458" s="9" t="str">
+      <c r="C458" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D458,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C459" s="9" t="str">
+      <c r="C459" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D459,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C460" s="9" t="str">
+      <c r="C460" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D460,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C461" s="9" t="str">
+      <c r="C461" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D461,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="462" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C462" s="9" t="str">
+      <c r="C462" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D462,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="463" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C463" s="9" t="str">
+      <c r="C463" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D463,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="464" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C464" s="9" t="str">
+      <c r="C464" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D464,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C465" s="9" t="str">
+      <c r="C465" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D465,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="466" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C466" s="9" t="str">
+      <c r="C466" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D466,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C467" s="9" t="str">
+      <c r="C467" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D467,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C468" s="9" t="str">
+      <c r="C468" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D468,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="469" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C469" s="9" t="str">
+      <c r="C469" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D469,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C470" s="9" t="str">
+      <c r="C470" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D470,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C471" s="9" t="str">
+      <c r="C471" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D471,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C472" s="9" t="str">
+      <c r="C472" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D472,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C473" s="9" t="str">
+      <c r="C473" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D473,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C474" s="9" t="str">
+      <c r="C474" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D474,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C475" s="9" t="str">
+      <c r="C475" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D475,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C476" s="9" t="str">
+      <c r="C476" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D476,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C477" s="9" t="str">
+      <c r="C477" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D477,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C478" s="9" t="str">
+      <c r="C478" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D478,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C479" s="9" t="str">
+      <c r="C479" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D479,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C480" s="9" t="str">
+      <c r="C480" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D480,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C481" s="9" t="str">
+      <c r="C481" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D481,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C482" s="9" t="str">
+      <c r="C482" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D482,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C483" s="9" t="str">
+      <c r="C483" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D483,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C484" s="9" t="str">
+      <c r="C484" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D484,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C485" s="9" t="str">
+      <c r="C485" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D485,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C486" s="9" t="str">
+      <c r="C486" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D486,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C487" s="9" t="str">
+      <c r="C487" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D487,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C488" s="9" t="str">
+      <c r="C488" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D488,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C489" s="9" t="str">
+      <c r="C489" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D489,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C490" s="9" t="str">
+      <c r="C490" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D490,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C491" s="9" t="str">
+      <c r="C491" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D491,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C492" s="9" t="str">
+      <c r="C492" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D492,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C493" s="9" t="str">
+      <c r="C493" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D493,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C494" s="9" t="str">
+      <c r="C494" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D494,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C495" s="9" t="str">
+      <c r="C495" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D495,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C496" s="9" t="str">
+      <c r="C496" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D496,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C497" s="9" t="str">
+      <c r="C497" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D497,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C498" s="9" t="str">
+      <c r="C498" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D498,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C499" s="9" t="str">
+      <c r="C499" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D499,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C500" s="9" t="str">
+      <c r="C500" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH(INDEX(OFFSET([2]Sheet1!$B$1,0,0,MaxCount),MATCH($D500,OFFSET([2]Sheet1!$A$1,0,0,MaxCount),0),1),OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
@@ -14193,10 +14180,10 @@
   <sheetFormatPr defaultColWidth="8.64453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="12" t="n">
+      <c r="B1" s="9" t="n">
         <v>2000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update new dragon girl
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Dragon_龙表.xlsx
+++ b/dragon-verse/Excels/Dragon_龙表.xlsx
@@ -129,10 +129,10 @@
     <t xml:space="preserve">0|0|0||0|0|75||1|1|1</t>
   </si>
   <si>
-    <t xml:space="preserve">2BC24957440AC3124367FDB1F4D964FB</t>
+    <t xml:space="preserve">91C494D2446711C104B6B0B67207DFDA</t>
   </si>
   <si>
-    <t xml:space="preserve">115D32374E1DD3F9F8E35180F601D2F7</t>
+    <t xml:space="preserve">FB3E449147E338443BAF48A103DA39E3</t>
   </si>
   <si>
     <t xml:space="preserve">EBD7C6BE429A512E1766AFACAFA30105</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">2B04CDB440F9BA9C0DEC58ACA3BC012F</t>
   </si>
   <si>
-    <t xml:space="preserve">442964B64CFE91D93BCD0C8F0C058117</t>
+    <t xml:space="preserve">5EB704B84A8F803191FA619D1FBEEA7B</t>
   </si>
   <si>
     <t xml:space="preserve">22D0B060433D9FBF41951DAFA2614DF2</t>
@@ -162,13 +162,13 @@
     <t xml:space="preserve">1ECFFBAF4EB541264762CC890F968872</t>
   </si>
   <si>
-    <t xml:space="preserve">5039CCD64DA4F2FDFFC8A1A6FF303806</t>
+    <t xml:space="preserve">C6F91F1643AE7170362762994B4C93EE</t>
   </si>
   <si>
     <t xml:space="preserve">37D752654AD6C496BCB97797B16B32E6</t>
   </si>
   <si>
-    <t xml:space="preserve">8BD91D2A4219B36F850259A31B81BFF7</t>
+    <t xml:space="preserve">C3D5A3A647168C57C91A84B5432B5A22</t>
   </si>
   <si>
     <t xml:space="preserve">E59CCE1B4B573E9E89526D8713A6DD02</t>
@@ -180,7 +180,7 @@
     <t xml:space="preserve">0|0|0||0|0|0||1|1|1</t>
   </si>
   <si>
-    <t xml:space="preserve">ABD1639E4D7779781D8E3495D0B6C695</t>
+    <t xml:space="preserve">13F7AAB9431A8B77B97C3390550C9BD3</t>
   </si>
   <si>
     <t xml:space="preserve">600933CC4486D357D0F9E48E8267286F</t>
@@ -213,13 +213,13 @@
     <t xml:space="preserve">0|0|0||0|0|78||1|1|1</t>
   </si>
   <si>
-    <t xml:space="preserve">5304164043CAE13137D6F7A1A96FE1A5</t>
+    <t xml:space="preserve">F404B1684A5454AA06913EABDD76436D</t>
   </si>
   <si>
     <t xml:space="preserve">0|0|0||0|0|86||1|1|1</t>
   </si>
   <si>
-    <t xml:space="preserve">AF3E8F5A4F90B0B95A2090956803BD32</t>
+    <t xml:space="preserve">FF96F37A4C33A4769B8E51966F6FD330</t>
   </si>
   <si>
     <t xml:space="preserve">41739B384717FFED535EC9B49EA34435</t>
@@ -231,7 +231,7 @@
     <t xml:space="preserve">C70CF68B4F6ACA4420195D9A091C1E32</t>
   </si>
   <si>
-    <t xml:space="preserve">4CFE3D0B44A54A6FCE0BACBB3CE63DAE</t>
+    <t xml:space="preserve">D06BEB6E400744FB99258D96E6E534C1</t>
   </si>
   <si>
     <t xml:space="preserve">A6DCDB104A426394C3ABD3ABA4FDF33F</t>
@@ -276,10 +276,10 @@
     <t xml:space="preserve">BFC127EE4493C33FA2D74E8955C7F430</t>
   </si>
   <si>
-    <t xml:space="preserve">5BD8296240A0DEFD9F6236AF55CA38AB</t>
+    <t xml:space="preserve">47B2A72D44B635A6E3940883F4949335</t>
   </si>
   <si>
-    <t xml:space="preserve">B4D3185544BCCC8845FD53A24EACDAC9</t>
+    <t xml:space="preserve">3C0747EB401208B7120423923964A1BB</t>
   </si>
   <si>
     <t xml:space="preserve">MaxLanItemCount</t>
@@ -654,7 +654,7 @@
   <dimension ref="A1:M2000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>